<commit_message>
Added plots and info
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1622846530014967</v>
+        <v>-0.8180139725122046</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4731087474115117</v>
+        <v>-0.4385921514182543</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3657438228083632</v>
+        <v>0.3092605588155036</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3857746683196281</v>
+        <v>0.3204530529485543</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4175420547424447</v>
+        <v>0.05413808103344353</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.8251205570085232</v>
+        <v>0.6752354387775248</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03794048968930203</v>
+        <v>0.3671020368216743</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05797133520056702</v>
+        <v>0.3782945309547249</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7370284911043179</v>
+        <v>-0.4699902090725725</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8344471688738579</v>
+        <v>0.4749393797381012</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3185438887263471</v>
+        <v>-0.02772933836605468</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2985130432150822</v>
+        <v>-0.01653684423300405</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.9680626756197157</v>
+        <v>0.5467038660876931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5910811539364782</v>
+        <v>-0.003159581291080071</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4135260594119031</v>
+        <v>0.1117741737900311</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.3934952139006381</v>
+        <v>0.1229666679230817</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2503405692908749</v>
+        <v>0.6094430382877407</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1771053472640649</v>
+        <v>-0.7914211707358625</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05848793404997667</v>
+        <v>-0.5088249777282632</v>
       </c>
       <c r="E6" t="n">
-        <v>0.07851877956124168</v>
+        <v>-0.4976324835952126</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7600530015463864</v>
+        <v>0.26044687922147</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.07244154556520233</v>
+        <v>-0.3999230529977498</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1146157844420802</v>
+        <v>-0.158933041270463</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0945849389308152</v>
+        <v>-0.1477405471374124</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2369212499464715</v>
+        <v>0.7398322420886418</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.4311768866808836</v>
+        <v>-0.1316216516568331</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.06142819571967535</v>
+        <v>0.04982596342212067</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.04139735020841036</v>
+        <v>0.0610184575551713</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.9811038610617198</v>
+        <v>0.8974631314321124</v>
       </c>
       <c r="C9" t="n">
-        <v>0.583345746732769</v>
+        <v>-0.537200097726501</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.414935800176957</v>
+        <v>-0.3502289269760306</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.394904954665692</v>
+        <v>-0.33903643284298</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02628556300377594</v>
+        <v>-0.9313160630050259</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.7750334311478777</v>
+        <v>-0.3640289314639717</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1658821633534185</v>
+        <v>0.3318350354796737</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1458513178421535</v>
+        <v>0.3430275296127244</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1564930361594288</v>
+        <v>0.649691719193338</v>
       </c>
       <c r="C11" t="n">
-        <v>0.08062373960182834</v>
+        <v>-0.6484078981324237</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1261991663226437</v>
+        <v>-0.409573208095256</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1462300118339087</v>
+        <v>-0.3983807139622054</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.6377229170602061</v>
+        <v>0.4629325164997189</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5803702719352131</v>
+        <v>0.2341588585026415</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.2652750699519408</v>
+        <v>0.2800519377065192</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.2452442244406758</v>
+        <v>0.2912444318395698</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6283433475952289</v>
+        <v>-0.7802850270179154</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3877578340431582</v>
+        <v>-0.6329263462578876</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8679716291039952</v>
+        <v>0.4024898801893085</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8880024746152602</v>
+        <v>0.4136823743223592</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.5404860798544953</v>
+        <v>-0.9702287095938849</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.2098792744941482</v>
+        <v>-0.6324332265968937</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.09503455670199887</v>
+        <v>0.5698195966884069</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.07500371119073387</v>
+        <v>0.5810120908214575</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1809552711198099</v>
+        <v>-0.5174014858441027</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.1466311145827239</v>
+        <v>-0.6791428774561667</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03703742197988574</v>
+        <v>0.2103699414174278</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05706826749115074</v>
+        <v>0.2215624355504784</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1985125946994473</v>
+        <v>0.8651340609620961</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4267478033787773</v>
+        <v>-0.5896833576772957</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3719527513524449</v>
+        <v>-0.4018149287499378</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3919835968637099</v>
+        <v>-0.3906224346168872</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7440218296412933</v>
+        <v>-0.9731474481201052</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.7049714418267861</v>
+        <v>-0.1696907746282261</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.07820632420351448</v>
+        <v>0.2115857261641171</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.05817547869224948</v>
+        <v>0.2227782202971677</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.1386767584905562</v>
+        <v>-0.08188190065829004</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.514993322738416</v>
+        <v>0.4823250952846854</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1053412058078259</v>
+        <v>0.1561047619386784</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.08531036029656087</v>
+        <v>0.167297256071729</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.565031600190349</v>
+        <v>0.1980134207212292</v>
       </c>
       <c r="C19" t="n">
-        <v>0.898924599563117</v>
+        <v>-0.8159509586557261</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.1588028645217318</v>
+        <v>-0.2998801834921427</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.1387720190104668</v>
+        <v>-0.2886876893590921</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5033923056375085</v>
+        <v>-0.7776166949092667</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1117957428977652</v>
+        <v>0.9256884273401516</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4455129009825243</v>
+        <v>-0.1482464041885797</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4655437464937893</v>
+        <v>-0.1370539100555291</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.2962445021283391</v>
+        <v>0.203215898749068</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.5014915693674558</v>
+        <v>0.5826619044744215</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.07721472249102826</v>
+        <v>0.4094657172915553</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.05718387697976327</v>
+        <v>0.420658211424606</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.4414321567087884</v>
+        <v>-0.4698230886947183</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8218774238785067</v>
+        <v>0.6746659055476678</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.06839815370919644</v>
+        <v>0.004334450532910206</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.04836730819793145</v>
+        <v>0.01552694466596083</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8585586611823954</v>
+        <v>0.7090078928075463</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7029380033004842</v>
+        <v>0.21635342230348</v>
       </c>
       <c r="D23" t="n">
-        <v>1.672081501475098</v>
+        <v>0.4001160235817616</v>
       </c>
       <c r="E23" t="n">
-        <v>1.692112346986363</v>
+        <v>0.4113085177148122</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.3649659373629783</v>
+        <v>0.1960798249591653</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.6961596848910681</v>
+        <v>0.04203233153523667</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0207871517501152</v>
+        <v>0.04850960301962629</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.0007563062388501983</v>
+        <v>0.05970209715267692</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.5705937265456349</v>
+        <v>0.4402964239131835</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.7609554344027534</v>
+        <v>0.727485269050417</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.1752080150517606</v>
+        <v>0.7657045903388009</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.1551771695404957</v>
+        <v>0.7768970844718516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed theta coefficients and regenerated
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.8180139725122046</v>
+        <v>-0.6231890030091449</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.4385921514182543</v>
+        <v>-0.3815599582472184</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3092605588155036</v>
+        <v>1.039208715109508</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3204530529485543</v>
+        <v>1.562018419371699</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05413808103344353</v>
+        <v>0.1313269621646771</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6752354387775248</v>
+        <v>0.8263615303988285</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3671020368216743</v>
+        <v>3.145821501937435</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3782945309547249</v>
+        <v>3.668631206199626</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4699902090725725</v>
+        <v>0.343234630204168</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4749393797381012</v>
+        <v>0.922789407056382</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.02772933836605468</v>
+        <v>4.810881543137723</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.01653684423300405</v>
+        <v>5.333691247399914</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5467038660876931</v>
+        <v>0.7125522396455506</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.003159581291080071</v>
+        <v>0.4815132279214041</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1117741737900311</v>
+        <v>2.567093677273756</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1229666679230817</v>
+        <v>3.089903381535947</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6094430382877407</v>
+        <v>0.8662106395267892</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.7914211707358625</v>
+        <v>0.1848282929284375</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5088249777282632</v>
+        <v>2.551152949613654</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.4976324835952126</v>
+        <v>3.073962653875845</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.26044687922147</v>
+        <v>-0.7743300267179998</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.3999230529977498</v>
+        <v>0.07101619575450724</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.158933041270463</v>
+        <v>1.675734724906242</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1477405471374124</v>
+        <v>2.198544429168433</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7398322420886418</v>
+        <v>0.6048556880868585</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1316216516568331</v>
+        <v>0.6871356504909893</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04982596342212067</v>
+        <v>3.311757838029258</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0610184575551713</v>
+        <v>3.834567542291449</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8974631314321124</v>
+        <v>0.6311408381149812</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.537200097726501</v>
+        <v>0.8219340074643868</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.3502289269760306</v>
+        <v>4.7030298689657</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.33903643284298</v>
+        <v>5.225839573227891</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.9313160630050259</v>
+        <v>-0.2162434898902577</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.3640289314639717</v>
+        <v>-0.8024443594015642</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3318350354796737</v>
+        <v>-2.307207602449695</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3430275296127244</v>
+        <v>-1.784397898187504</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.649691719193338</v>
+        <v>0.2977985744636613</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.6484078981324237</v>
+        <v>-0.4769871861722883</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.409573208095256</v>
+        <v>-0.4137742482290986</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.3983807139622054</v>
+        <v>0.1090354560330925</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4629325164997189</v>
+        <v>0.623077212741084</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2341588585026415</v>
+        <v>0.4963231194350934</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2800519377065192</v>
+        <v>2.221809807309105</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2912444318395698</v>
+        <v>2.744619511571297</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.7802850270179154</v>
+        <v>0.5205295124310321</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.6329263462578876</v>
+        <v>0.09129625313229872</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4024898801893085</v>
+        <v>0.926196165218044</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4136823743223592</v>
+        <v>1.449005869480235</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.9702287095938849</v>
+        <v>-0.916138814832975</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.6324332265968937</v>
+        <v>0.2995899633392989</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5698195966884069</v>
+        <v>2.325232726393821</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5810120908214575</v>
+        <v>2.848042430656012</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5174014858441027</v>
+        <v>-0.6876339652659114</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.6791428774561667</v>
+        <v>-0.3308805041004506</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2103699414174278</v>
+        <v>1.374015682954193</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2215624355504784</v>
+        <v>1.896825387216384</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8651340609620961</v>
+        <v>-0.2690791256533465</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.5896833576772957</v>
+        <v>0.4919033169845433</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.4018149287499378</v>
+        <v>0.7264555764250926</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.3906224346168872</v>
+        <v>1.249265280687284</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.9731474481201052</v>
+        <v>-0.4749217012840903</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1696907746282261</v>
+        <v>0.994134128454679</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2115857261641171</v>
+        <v>5.267794549091613</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2227782202971677</v>
+        <v>5.790604253353805</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.08188190065829004</v>
+        <v>0.5228567667030581</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4823250952846854</v>
+        <v>0.03072945381546499</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1561047619386784</v>
+        <v>0.8918028393245876</v>
       </c>
       <c r="E18" t="n">
-        <v>0.167297256071729</v>
+        <v>1.414612543586779</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1980134207212292</v>
+        <v>-0.05567193566994177</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.8159509586557261</v>
+        <v>-0.8750665542320568</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.2998801834921427</v>
+        <v>-3.308858726275794</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2886876893590921</v>
+        <v>-2.786049022013603</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.7776166949092667</v>
+        <v>-0.5499603893133345</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9256884273401516</v>
+        <v>-0.9715321191867849</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1482464041885797</v>
+        <v>-3.201111049687445</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.1370539100555291</v>
+        <v>-2.678301345425254</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.203215898749068</v>
+        <v>-0.3722712987954699</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5826619044744215</v>
+        <v>-0.687399935006419</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4094657172915553</v>
+        <v>-1.011104747457896</v>
       </c>
       <c r="E21" t="n">
-        <v>0.420658211424606</v>
+        <v>-0.4882950431957049</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.4698230886947183</v>
+        <v>-0.8036632759173747</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6746659055476678</v>
+        <v>0.6512951215389555</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004334450532910206</v>
+        <v>2.822732927983922</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01552694466596083</v>
+        <v>3.345542632246112</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.7090078928075463</v>
+        <v>0.5773802583911078</v>
       </c>
       <c r="C23" t="n">
-        <v>0.21635342230348</v>
+        <v>0.3034691942391716</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4001160235817616</v>
+        <v>1.412353090447157</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4113085177148122</v>
+        <v>1.935162794709348</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1960798249591653</v>
+        <v>0.9406693238294122</v>
       </c>
       <c r="C24" t="n">
-        <v>0.04203233153523667</v>
+        <v>-0.006699004185547475</v>
       </c>
       <c r="D24" t="n">
-        <v>0.04850960301962629</v>
+        <v>2.741674799129028</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05970209715267692</v>
+        <v>3.264484503391219</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.4402964239131835</v>
+        <v>-0.8146686208556893</v>
       </c>
       <c r="C25" t="n">
-        <v>0.727485269050417</v>
+        <v>0.5631427997865806</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7657045903388009</v>
+        <v>2.431787370368446</v>
       </c>
       <c r="E25" t="n">
-        <v>0.7768970844718516</v>
+        <v>2.954597074630637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FULL UPDATE Copy from collab notebook
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6231890030091449</v>
+        <v>0.2383949248408106</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3815599582472184</v>
+        <v>0.7472224567323638</v>
       </c>
       <c r="D2" t="n">
-        <v>1.039208715109508</v>
+        <v>3.943587850293786</v>
       </c>
       <c r="E2" t="n">
-        <v>1.562018419371699</v>
+        <v>4.505406420336354</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1313269621646771</v>
+        <v>-0.2202018404700252</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8263615303988285</v>
+        <v>0.7056791448964408</v>
       </c>
       <c r="D3" t="n">
-        <v>3.145821501937435</v>
+        <v>2.682566340584926</v>
       </c>
       <c r="E3" t="n">
-        <v>3.668631206199626</v>
+        <v>2.526179711573022</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.343234630204168</v>
+        <v>0.5352351834364462</v>
       </c>
       <c r="C4" t="n">
-        <v>0.922789407056382</v>
+        <v>0.4193852692103233</v>
       </c>
       <c r="D4" t="n">
-        <v>4.810881543137723</v>
+        <v>3.925510686800984</v>
       </c>
       <c r="E4" t="n">
-        <v>5.333691247399914</v>
+        <v>4.658091882852515</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7125522396455506</v>
+        <v>-0.2526107621502742</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4815132279214041</v>
+        <v>-0.1622500265911551</v>
       </c>
       <c r="D5" t="n">
-        <v>2.567093677273756</v>
+        <v>0.6487093939848017</v>
       </c>
       <c r="E5" t="n">
-        <v>3.089903381535947</v>
+        <v>2.371363058817952</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8662106395267892</v>
+        <v>0.2980337708510654</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1848282929284375</v>
+        <v>0.9058999966466461</v>
       </c>
       <c r="D6" t="n">
-        <v>2.551152949613654</v>
+        <v>6.752630535318094</v>
       </c>
       <c r="E6" t="n">
-        <v>3.073962653875845</v>
+        <v>6.487786633930948</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7743300267179998</v>
+        <v>0.7849677282725567</v>
       </c>
       <c r="C7" t="n">
-        <v>0.07101619575450724</v>
+        <v>-0.3609247456704967</v>
       </c>
       <c r="D7" t="n">
-        <v>1.675734724906242</v>
+        <v>5.308403828860486</v>
       </c>
       <c r="E7" t="n">
-        <v>2.198544429168433</v>
+        <v>5.043578497128229</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6048556880868585</v>
+        <v>0.7402292915633248</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6871356504909893</v>
+        <v>-0.1470334276963767</v>
       </c>
       <c r="D8" t="n">
-        <v>3.311757838029258</v>
+        <v>5.29878589365986</v>
       </c>
       <c r="E8" t="n">
-        <v>3.834567542291449</v>
+        <v>7.084986428560254</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6311408381149812</v>
+        <v>0.5000916116287533</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8219340074643868</v>
+        <v>0.9894397009368099</v>
       </c>
       <c r="D9" t="n">
-        <v>4.7030298689657</v>
+        <v>10.42005771490263</v>
       </c>
       <c r="E9" t="n">
-        <v>5.225839573227891</v>
+        <v>11.2880802576868</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2162434898902577</v>
+        <v>-0.2940049544438035</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.8024443594015642</v>
+        <v>-0.4543519506929634</v>
       </c>
       <c r="D10" t="n">
-        <v>-2.307207602449695</v>
+        <v>0.4001556656665962</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.784397898187504</v>
+        <v>-0.1308528159291008</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2977985744636613</v>
+        <v>-0.6768553285529779</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.4769871861722883</v>
+        <v>-0.33547294328508</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.4137742482290986</v>
+        <v>4.669948032657382</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1090354560330925</v>
+        <v>5.283621522735703</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.623077212741084</v>
+        <v>0.8679762954857695</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4963231194350934</v>
+        <v>-0.1303801466926966</v>
       </c>
       <c r="D12" t="n">
-        <v>2.221809807309105</v>
+        <v>7.365740047706666</v>
       </c>
       <c r="E12" t="n">
-        <v>2.744619511571297</v>
+        <v>6.841582111134974</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5205295124310321</v>
+        <v>0.2087442628646587</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09129625313229872</v>
+        <v>0.6245897484059622</v>
       </c>
       <c r="D13" t="n">
-        <v>0.926196165218044</v>
+        <v>2.485455365594244</v>
       </c>
       <c r="E13" t="n">
-        <v>1.449005869480235</v>
+        <v>1.958682326028363</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.916138814832975</v>
+        <v>-0.9161027300281184</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2995899633392989</v>
+        <v>0.5563364874951686</v>
       </c>
       <c r="D14" t="n">
-        <v>2.325232726393821</v>
+        <v>8.542485808011877</v>
       </c>
       <c r="E14" t="n">
-        <v>2.848042430656012</v>
+        <v>8.816162119812896</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.6876339652659114</v>
+        <v>-0.4779641748051917</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.3308805041004506</v>
+        <v>-0.7713405236652651</v>
       </c>
       <c r="D15" t="n">
-        <v>1.374015682954193</v>
+        <v>-0.3155374726161347</v>
       </c>
       <c r="E15" t="n">
-        <v>1.896825387216384</v>
+        <v>-2.479591717150677</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2690791256533465</v>
+        <v>-0.2694790629375337</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4919033169845433</v>
+        <v>0.01406229217945465</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7264555764250926</v>
+        <v>0.6930884554396732</v>
       </c>
       <c r="E16" t="n">
-        <v>1.249265280687284</v>
+        <v>-1.257914680324575</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4749217012840903</v>
+        <v>-0.5036926508312598</v>
       </c>
       <c r="C17" t="n">
-        <v>0.994134128454679</v>
+        <v>0.2449159603378641</v>
       </c>
       <c r="D17" t="n">
-        <v>5.267794549091613</v>
+        <v>2.367297434616092</v>
       </c>
       <c r="E17" t="n">
-        <v>5.790604253353805</v>
+        <v>1.731310773644529</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5228567667030581</v>
+        <v>0.8437022691231302</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03072945381546499</v>
+        <v>0.6580720897494881</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8918028393245876</v>
+        <v>10.37383416926501</v>
       </c>
       <c r="E18" t="n">
-        <v>1.414612543586779</v>
+        <v>9.2282510843634</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.05567193566994177</v>
+        <v>-0.02522713199040472</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.8750665542320568</v>
+        <v>0.4967204172120905</v>
       </c>
       <c r="D19" t="n">
-        <v>-3.308858726275794</v>
+        <v>0.8863466252612221</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.786049022013603</v>
+        <v>1.241782414573985</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.5499603893133345</v>
+        <v>0.9530534962439339</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.9715321191867849</v>
+        <v>0.2974198651668136</v>
       </c>
       <c r="D20" t="n">
-        <v>-3.201111049687445</v>
+        <v>9.959236452503314</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.678301345425254</v>
+        <v>8.93219749140084</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3722712987954699</v>
+        <v>-0.770616894872048</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.687399935006419</v>
+        <v>-0.2115879263803888</v>
       </c>
       <c r="D21" t="n">
-        <v>-1.011104747457896</v>
+        <v>6.100081239627848</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.4882950431957049</v>
+        <v>4.502666627743261</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.8036632759173747</v>
+        <v>0.01821673272617774</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6512951215389555</v>
+        <v>-0.6145031556205331</v>
       </c>
       <c r="D22" t="n">
-        <v>2.822732927983922</v>
+        <v>-1.703014142259259</v>
       </c>
       <c r="E22" t="n">
-        <v>3.345542632246112</v>
+        <v>-0.04526251479247279</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.5773802583911078</v>
+        <v>0.3335423626506677</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3034691942391716</v>
+        <v>0.4207305198267379</v>
       </c>
       <c r="D23" t="n">
-        <v>1.412353090447157</v>
+        <v>1.989922115567548</v>
       </c>
       <c r="E23" t="n">
-        <v>1.935162794709348</v>
+        <v>1.734553273105799</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.9406693238294122</v>
+        <v>-0.1301503276917138</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.006699004185547475</v>
+        <v>0.4589077780388409</v>
       </c>
       <c r="D24" t="n">
-        <v>2.741674799129028</v>
+        <v>0.7593229448914218</v>
       </c>
       <c r="E24" t="n">
-        <v>3.264484503391219</v>
+        <v>0.835702084010603</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,1308 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.8146686208556893</v>
+        <v>-0.8079413866480227</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5631427997865806</v>
+        <v>0.5139500613006649</v>
       </c>
       <c r="D25" t="n">
-        <v>2.431787370368446</v>
+        <v>6.618110828883571</v>
       </c>
       <c r="E25" t="n">
-        <v>2.954597074630637</v>
+        <v>5.006620631157949</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.8204610279399496</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.2268088114858982</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6.337079755705422</v>
+      </c>
+      <c r="E26" t="n">
+        <v>5.721344685555933</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-0.09132612899372794</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.01502864370079804</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.07305361473415382</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.1985148490445161</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.8043964908147241</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.4357975579673012</v>
+      </c>
+      <c r="D28" t="n">
+        <v>5.226923769619499</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.925069248512358</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.2821140949083631</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-0.1960126508799476</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.6411809480962762</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.066121776045704</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.4232561955622904</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.6466520413808639</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4.33867083524015</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.659306319780504</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.2828996832111237</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.7164080978719944</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3.879424200499004</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.549498096308638</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.6755128141969458</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-0.3612097941293129</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3.776706581427143</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.096134170879717</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.497196867192925</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.1357403609524448</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.687827871160612</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.782884504101614</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.2069121000286771</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.2042785834362983</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.6134521058297779</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.5981857973184564</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1391055923733706</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.1897533419372412</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.3270073049665112</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.8693379934751093</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.07919738317726632</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-0.253531895386474</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-0.0444689585981396</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.8858870691334738</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-0.5117598320535051</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-0.3763083658066984</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2.542315560377665</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.161455704635326</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.6532698979742728</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.3187436735522757</v>
+      </c>
+      <c r="D38" t="n">
+        <v>5.007953235628285</v>
+      </c>
+      <c r="E38" t="n">
+        <v>5.244192621134316</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-0.06167808181044032</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-0.9299792402237905</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-5.576527153801635</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-7.793051607713017</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.5614569134839866</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.8934003961117531</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-2.875629260017932</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-4.377900903012026</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-0.4933161491432858</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.5454499185345714</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.731931059493485</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1.954594934404862</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.8324883562683414</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.5332165369331476</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5.011274283556021</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5.846531816449119</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.3299122523917237</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-0.6269844305098482</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-1.080300613409902</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-0.8864710595203338</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>-0.5125016184881652</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-0.8693023313266497</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-1.219004118526207</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-1.349810442939055</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.4562622404139616</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.6388742054740928</v>
+      </c>
+      <c r="D45" t="n">
+        <v>4.599595707382056</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4.259026294038439</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-0.04638371212631975</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.05102603886394363</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.01817514597978535</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-1.654136998477944</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.2452970443332452</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0419972644457729</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.6515579548121512</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-0.1626363687480108</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.3903293580024056</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.2741915455747761</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.948370156599979</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1.427355375688469</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.9859017774955614</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-0.2910116309888502</v>
+      </c>
+      <c r="D49" t="n">
+        <v>9.043178513586357</v>
+      </c>
+      <c r="E49" t="n">
+        <v>10.23885794791304</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-0.4789146635581092</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.8512696276024665</v>
+      </c>
+      <c r="D50" t="n">
+        <v>5.833624244021098</v>
+      </c>
+      <c r="E50" t="n">
+        <v>6.222280647136433</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>-0.442693832403426</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.4737219774513339</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2.287617483984073</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.2934953253768504</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.2853156761554017</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.3207390593974342</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.288648534035373</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1.655210249974612</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>-0.3794695885724375</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.4998203120818865</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.946730519903219</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1.511175432896601</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-0.5969955897002779</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-0.2509440905329223</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3.668249599735322</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.902603306114113</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.02303638816221021</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.005727854690717349</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.008448389697878651</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.7002972042367906</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-0.3825845250099931</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.2241663919120507</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.355193614076288</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.521326437012273</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>-0.6398992139946655</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.7239605939605747</v>
+      </c>
+      <c r="D57" t="n">
+        <v>5.832682770535864</v>
+      </c>
+      <c r="E57" t="n">
+        <v>6.886025949221378</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.02245435673427076</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-0.4090263866980317</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-0.5310022732723614</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-1.480216194384341</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.7709437818589016</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.2046833202650513</v>
+      </c>
+      <c r="D59" t="n">
+        <v>6.416731352824671</v>
+      </c>
+      <c r="E59" t="n">
+        <v>6.06699045297907</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>-0.01648717495557883</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-0.008535681113036597</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0004930890693058833</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.375175280446961</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.4341100716521393</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.5996639989701711</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2.889891827157039</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.993301836735495</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.790239389326461</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-0.6790142690955754</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2.991271766442376</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.449292071530421</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>-5.019450631205125e-05</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.5168177912309293</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.01792140305682</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.8079280695621055</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>-0.08551266788755041</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-0.878264967499401</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-4.615191840823298</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-5.866534347003291</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.9082000566132071</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-0.767857647085354</v>
+      </c>
+      <c r="D65" t="n">
+        <v>3.698440027840316</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2.345446377584387</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-0.0853154548894528</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-0.4960643257333781</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-0.7552067258768602</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.163817008181804</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.8919100405540348</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-0.0693983783984109</v>
+      </c>
+      <c r="D67" t="n">
+        <v>7.911152525965866</v>
+      </c>
+      <c r="E67" t="n">
+        <v>9.445155189000353</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>-0.2343004083501838</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.5469373059077962</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.469212609833273</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.387764108135477</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-0.6531702354534958</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.7136308562528624</v>
+      </c>
+      <c r="D69" t="n">
+        <v>5.884125260809406</v>
+      </c>
+      <c r="E69" t="n">
+        <v>7.019191403512252</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.008184855241341937</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.8056725469705073</v>
+      </c>
+      <c r="D70" t="n">
+        <v>3.728010957239567</v>
+      </c>
+      <c r="E70" t="n">
+        <v>4.137046683796659</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-0.1586201901567554</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.1403083560679679</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.2245961867128068</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.5050795349094578</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>-0.9798303335318344</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.2845541581939639</v>
+      </c>
+      <c r="D72" t="n">
+        <v>9.134802196628064</v>
+      </c>
+      <c r="E72" t="n">
+        <v>9.543565991811917</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.830351451134915</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-0.1291338350183866</v>
+      </c>
+      <c r="D73" t="n">
+        <v>6.735430509374736</v>
+      </c>
+      <c r="E73" t="n">
+        <v>8.475057816562721</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.4487369574505953</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-0.4739534750091063</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.8405105618473387</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.799988797083799</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-0.06387243330467873</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.6959837400658753</v>
+      </c>
+      <c r="D75" t="n">
+        <v>2.375009005848729</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4.144730798567048</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-0.6359475884248171</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.1729858134349052</v>
+      </c>
+      <c r="D76" t="n">
+        <v>3.81421245631046</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.8510968709519848</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-0.9816503712409568</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-0.6818373278733265</v>
+      </c>
+      <c r="D77" t="n">
+        <v>8.589764037682631</v>
+      </c>
+      <c r="E77" t="n">
+        <v>9.519393457185101</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.005818402290541869</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-0.2268987264580853</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-0.1061799113775859</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-0.007723567608252518</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.3714233640354083</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.01098126124406629</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.407430700341795</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.06923240046941</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2727511091622636</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.04483500767949589</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.8007787677197491</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.9045666464154578</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-0.08111021555299858</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-0.9389552859882375</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-5.678624389679264</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-7.926704334034866</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.1427156067511872</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.439998439272447</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.9838197918952118</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.7353554685912786</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.4793182136338827</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.3536845252602541</v>
+      </c>
+      <c r="D83" t="n">
+        <v>3.029518215738307</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3.433437598857669</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.9969029160968941</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.6255708438592831</v>
+      </c>
+      <c r="D84" t="n">
+        <v>13.06133977094095</v>
+      </c>
+      <c r="E84" t="n">
+        <v>14.73294166482201</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-0.08708884175221732</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-0.3540058096164784</v>
+      </c>
+      <c r="D85" t="n">
+        <v>-0.2171532267401139</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-0.8033532195548253</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.5004128935183039</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.7603139795761495</v>
+      </c>
+      <c r="D86" t="n">
+        <v>-1.359443325887403</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.273906336680136</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-0.4275268192483859</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.7594320984457046</v>
+      </c>
+      <c r="D87" t="n">
+        <v>-0.7074976283550021</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-1.27502006158246</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.8689447674681618</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-0.6162873730613621</v>
+      </c>
+      <c r="D88" t="n">
+        <v>4.866371157843714</v>
+      </c>
+      <c r="E88" t="n">
+        <v>5.901755202497033</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.8768918058528758</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.5672282689567938</v>
+      </c>
+      <c r="D89" t="n">
+        <v>10.10613160804239</v>
+      </c>
+      <c r="E89" t="n">
+        <v>10.47797218719483</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.4832469272882356</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.702902249541733</v>
+      </c>
+      <c r="D90" t="n">
+        <v>5.56422968734362</v>
+      </c>
+      <c r="E90" t="n">
+        <v>4.965033714485713</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>-0.4251971581236265</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-0.3648456619531026</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1.699226365844701</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2.279767857511527</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.05043595275522295</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-0.7452970013161559</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-3.017146241737718</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-2.907344719821511</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.3796988753079562</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.8019949572771687</v>
+      </c>
+      <c r="D93" t="n">
+        <v>5.779794051860228</v>
+      </c>
+      <c r="E93" t="n">
+        <v>6.87539952265457</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-0.160349168749178</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.4263802258935261</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.6895940003965425</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-0.1044773239355733</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-0.3302712791928246</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.9527075822396023</v>
+      </c>
+      <c r="D95" t="n">
+        <v>6.576817749958067</v>
+      </c>
+      <c r="E95" t="n">
+        <v>6.206208864459946</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-0.7134113439807968</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-0.6124596480862541</v>
+      </c>
+      <c r="D96" t="n">
+        <v>4.222677140255817</v>
+      </c>
+      <c r="E96" t="n">
+        <v>3.77917529808109</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.6750039375280479</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-0.3982867363297973</v>
+      </c>
+      <c r="D97" t="n">
+        <v>3.604016591173855</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1.948678464786875</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.9084212572536554</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-0.4534948211072669</v>
+      </c>
+      <c r="D98" t="n">
+        <v>6.821003333098134</v>
+      </c>
+      <c r="E98" t="n">
+        <v>7.155936150317995</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.2192381915177724</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.9907954148719071</v>
+      </c>
+      <c r="D99" t="n">
+        <v>7.844575062155222</v>
+      </c>
+      <c r="E99" t="n">
+        <v>8.139846897735197</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-0.655308769228488</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.4329103861408079</v>
+      </c>
+      <c r="D100" t="n">
+        <v>4.272602445460303</v>
+      </c>
+      <c r="E100" t="n">
+        <v>4.278386123822247</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-0.6612794202262902</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-0.2246659564347393</v>
+      </c>
+      <c r="D101" t="n">
+        <v>4.502064353400205</v>
+      </c>
+      <c r="E101" t="n">
+        <v>4.236729840533546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added exit statement for menu
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2383949248408106</v>
+        <v>-0.7883267274870609</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7472224567323638</v>
+        <v>0.800085954409169</v>
       </c>
       <c r="D2" t="n">
-        <v>3.943587850293786</v>
+        <v>14.08421954069435</v>
       </c>
       <c r="E2" t="n">
-        <v>4.505406420336354</v>
+        <v>20.84790550155498</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2202018404700252</v>
+        <v>0.4067218946723166</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7056791448964408</v>
+        <v>-0.8024105160763451</v>
       </c>
       <c r="D3" t="n">
-        <v>2.682566340584926</v>
+        <v>69.79870575383211</v>
       </c>
       <c r="E3" t="n">
-        <v>2.526179711573022</v>
+        <v>67.91598043374525</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5352351834364462</v>
+        <v>0.3217520894772643</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4193852692103233</v>
+        <v>-0.7404537878180328</v>
       </c>
       <c r="D4" t="n">
-        <v>3.925510686800984</v>
+        <v>52.09877729250569</v>
       </c>
       <c r="E4" t="n">
-        <v>4.658091882852515</v>
+        <v>60.91825997807945</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2526107621502742</v>
+        <v>0.6570128138945719</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1622500265911551</v>
+        <v>0.2581283720985377</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6487093939848017</v>
+        <v>40.69021367644633</v>
       </c>
       <c r="E5" t="n">
-        <v>2.371363058817952</v>
+        <v>61.42909457063656</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2980337708510654</v>
+        <v>-0.2977538290088548</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9058999966466461</v>
+        <v>0.3968395867426517</v>
       </c>
       <c r="D6" t="n">
-        <v>6.752630535318094</v>
+        <v>3.216949784596996</v>
       </c>
       <c r="E6" t="n">
-        <v>6.487786633930948</v>
+        <v>0.02851659077062552</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7849677282725567</v>
+        <v>-0.8379969398586182</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.3609247456704967</v>
+        <v>0.6350416081076644</v>
       </c>
       <c r="D7" t="n">
-        <v>5.308403828860486</v>
+        <v>47.25458515088006</v>
       </c>
       <c r="E7" t="n">
-        <v>5.043578497128229</v>
+        <v>44.06637551554883</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7402292915633248</v>
+        <v>0.745702201662465</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1470334276963767</v>
+        <v>0.9992229584316992</v>
       </c>
       <c r="D8" t="n">
-        <v>5.29878589365986</v>
+        <v>-47.71101254850895</v>
       </c>
       <c r="E8" t="n">
-        <v>7.084986428560254</v>
+        <v>-26.2070962926398</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5000916116287533</v>
+        <v>-0.7525429745663264</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9894397009368099</v>
+        <v>0.8592508216668169</v>
       </c>
       <c r="D9" t="n">
-        <v>10.42005771490263</v>
+        <v>-3.563637588771424</v>
       </c>
       <c r="E9" t="n">
-        <v>11.2880802576868</v>
+        <v>6.886411945716119</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2940049544438035</v>
+        <v>-0.9036575038632009</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.4543519506929634</v>
+        <v>0.1333062515789742</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4001556656665962</v>
+        <v>81.94807664600607</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1308528159291008</v>
+        <v>75.55531071839602</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.6768553285529779</v>
+        <v>-0.5874227318484027</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.33547294328508</v>
+        <v>0.7630646847948557</v>
       </c>
       <c r="D11" t="n">
-        <v>4.669948032657382</v>
+        <v>-7.665474409358794</v>
       </c>
       <c r="E11" t="n">
-        <v>5.283621522735703</v>
+        <v>-0.2775114784065682</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8679762954857695</v>
+        <v>-0.3067545647977408</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.1303801466926966</v>
+        <v>-0.004970795907636161</v>
       </c>
       <c r="D12" t="n">
-        <v>7.365740047706666</v>
+        <v>9.371051976924006</v>
       </c>
       <c r="E12" t="n">
-        <v>6.841582111134974</v>
+        <v>3.06075917796043</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2087442628646587</v>
+        <v>0.5644116894058673</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6245897484059622</v>
+        <v>0.8041349689470894</v>
       </c>
       <c r="D13" t="n">
-        <v>2.485455365594244</v>
+        <v>-22.27443032219932</v>
       </c>
       <c r="E13" t="n">
-        <v>1.958682326028363</v>
+        <v>-28.61620612359669</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.9161027300281184</v>
+        <v>-0.8997496845279418</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5563364874951686</v>
+        <v>0.5039019772166953</v>
       </c>
       <c r="D14" t="n">
-        <v>8.542485808011877</v>
+        <v>70.38735488914189</v>
       </c>
       <c r="E14" t="n">
-        <v>8.816162119812896</v>
+        <v>73.68212072041089</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.4779641748051917</v>
+        <v>-0.8430710240680073</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.7713405236652651</v>
+        <v>0.9810635957087623</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.3155374726161347</v>
+        <v>-19.1997700282388</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.479591717150677</v>
+        <v>-45.25263494366892</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2694790629375337</v>
+        <v>0.8514766189779066</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01406229217945465</v>
+        <v>0.08345352652200022</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6930884554396732</v>
+        <v>72.18132151395056</v>
       </c>
       <c r="E16" t="n">
-        <v>-1.257914680324575</v>
+        <v>48.69336076896509</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.5036926508312598</v>
+        <v>0.5129950434980493</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2449159603378641</v>
+        <v>-0.2376006257412293</v>
       </c>
       <c r="D17" t="n">
-        <v>2.367297434616092</v>
+        <v>28.29472255908012</v>
       </c>
       <c r="E17" t="n">
-        <v>1.731310773644529</v>
+        <v>20.6381332623218</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8437022691231302</v>
+        <v>-0.9895408966379746</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6580720897494881</v>
+        <v>0.9365270184260108</v>
       </c>
       <c r="D18" t="n">
-        <v>10.37383416926501</v>
+        <v>20.4062969249014</v>
       </c>
       <c r="E18" t="n">
-        <v>9.2282510843634</v>
+        <v>6.61471964086584</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.02522713199040472</v>
+        <v>0.7831680939175434</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4967204172120905</v>
+        <v>0.6101219877323796</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8863466252612221</v>
+        <v>36.37369475628973</v>
       </c>
       <c r="E19" t="n">
-        <v>1.241782414573985</v>
+        <v>40.65275598059209</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9530534962439339</v>
+        <v>0.199814456183109</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2974198651668136</v>
+        <v>-0.3380624954873288</v>
       </c>
       <c r="D20" t="n">
-        <v>9.959236452503314</v>
+        <v>8.180095270900543</v>
       </c>
       <c r="E20" t="n">
-        <v>8.93219749140084</v>
+        <v>-4.184339393370797</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.770616894872048</v>
+        <v>-0.3198043211807147</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.2115879263803888</v>
+        <v>-0.003899044295286869</v>
       </c>
       <c r="D21" t="n">
-        <v>6.100081239627848</v>
+        <v>10.18888131950782</v>
       </c>
       <c r="E21" t="n">
-        <v>4.502666627743261</v>
+        <v>-9.042257272544731</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.01821673272617774</v>
+        <v>0.01526721880575921</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.6145031556205331</v>
+        <v>-0.9229619526462962</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.703014142259259</v>
+        <v>78.62631764166164</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.04526251479247279</v>
+        <v>98.583848430367</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3335423626506677</v>
+        <v>0.600864302517591</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4207305198267379</v>
+        <v>-0.6901452826030117</v>
       </c>
       <c r="D23" t="n">
-        <v>1.989922115567548</v>
+        <v>71.03993630897288</v>
       </c>
       <c r="E23" t="n">
-        <v>1.734553273105799</v>
+        <v>67.96557254333784</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.1301503276917138</v>
+        <v>0.7070253064025853</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4589077780388409</v>
+        <v>0.5862124932915631</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7593229448914218</v>
+        <v>27.90056248807203</v>
       </c>
       <c r="E24" t="n">
-        <v>0.835702084010603</v>
+        <v>28.82008444499824</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.8079413866480227</v>
+        <v>-0.5659865789389336</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5139500613006649</v>
+        <v>-0.2908965280207036</v>
       </c>
       <c r="D25" t="n">
-        <v>6.618110828883571</v>
+        <v>33.58676419096425</v>
       </c>
       <c r="E25" t="n">
-        <v>5.006620631157949</v>
+        <v>14.1861708186315</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8204610279399496</v>
+        <v>0.1704155445933895</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.2268088114858982</v>
+        <v>-0.5668478282546454</v>
       </c>
       <c r="D26" t="n">
-        <v>6.337079755705422</v>
+        <v>21.56125473815938</v>
       </c>
       <c r="E26" t="n">
-        <v>5.721344685555933</v>
+        <v>14.14847262014558</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.09132612899372794</v>
+        <v>0.137885576416714</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01502864370079804</v>
+        <v>-0.3505592017192578</v>
       </c>
       <c r="D27" t="n">
-        <v>0.07305361473415382</v>
+        <v>6.429744658691332</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1985148490445161</v>
+        <v>7.940161783338793</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8043964908147241</v>
+        <v>0.7598851424733513</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.4357975579673012</v>
+        <v>-0.7837352789227821</v>
       </c>
       <c r="D28" t="n">
-        <v>5.226923769619499</v>
+        <v>108.85813509274</v>
       </c>
       <c r="E28" t="n">
-        <v>3.925069248512358</v>
+        <v>93.18521928501201</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2821140949083631</v>
+        <v>0.006121628562932635</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.1960126508799476</v>
+        <v>-0.8085434330345842</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6411809480962762</v>
+        <v>52.80617242694299</v>
       </c>
       <c r="E29" t="n">
-        <v>1.066121776045704</v>
+        <v>57.92199889736433</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.4232561955622904</v>
+        <v>-0.5778692615891516</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6466520413808639</v>
+        <v>-0.5221182061656144</v>
       </c>
       <c r="D30" t="n">
-        <v>4.33867083524015</v>
+        <v>46.00803906582677</v>
       </c>
       <c r="E30" t="n">
-        <v>3.659306319780504</v>
+        <v>37.82922746981076</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2828996832111237</v>
+        <v>0.7461202387056165</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7164080978719944</v>
+        <v>0.2742859745515567</v>
       </c>
       <c r="D31" t="n">
-        <v>3.879424200499004</v>
+        <v>52.68480002550503</v>
       </c>
       <c r="E31" t="n">
-        <v>3.549498096308638</v>
+        <v>48.71284772982933</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.6755128141969458</v>
+        <v>0.5372641962823503</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.3612097941293129</v>
+        <v>0.2251356548244388</v>
       </c>
       <c r="D32" t="n">
-        <v>3.776706581427143</v>
+        <v>27.19561101253748</v>
       </c>
       <c r="E32" t="n">
-        <v>3.096134170879717</v>
+        <v>19.00225767033677</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.497196867192925</v>
+        <v>-0.8949254046015516</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1357403609524448</v>
+        <v>-0.08774207566073966</v>
       </c>
       <c r="D33" t="n">
-        <v>2.687827871160612</v>
+        <v>79.66581791401077</v>
       </c>
       <c r="E33" t="n">
-        <v>4.782884504101614</v>
+        <v>104.8880264543183</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.2069121000286771</v>
+        <v>0.05914426922634908</v>
       </c>
       <c r="C34" t="n">
-        <v>0.2042785834362983</v>
+        <v>-0.1792469726263153</v>
       </c>
       <c r="D34" t="n">
-        <v>0.6134521058297779</v>
+        <v>0.9667124958665121</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5981857973184564</v>
+        <v>0.7829227066746588</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1391055923733706</v>
+        <v>-0.3202157862062349</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1897533419372412</v>
+        <v>0.6992849473576421</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3270073049665112</v>
+        <v>-22.7836623123874</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.8693379934751093</v>
+        <v>-37.18636156598828</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.07919738317726632</v>
+        <v>-0.3451356101837937</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.253531895386474</v>
+        <v>-0.7701527628759548</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.0444689585981396</v>
+        <v>56.15177170947156</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8858870691334738</v>
+        <v>67.35224876542505</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.5117598320535051</v>
+        <v>-0.02303954825946541</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.3763083658066984</v>
+        <v>-0.1628023249015498</v>
       </c>
       <c r="D37" t="n">
-        <v>2.542315560377665</v>
+        <v>0.4472444320869069</v>
       </c>
       <c r="E37" t="n">
-        <v>1.161455704635326</v>
+        <v>-16.17680987692755</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6532698979742728</v>
+        <v>-0.8379980196241088</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3187436735522757</v>
+        <v>0.471818754638156</v>
       </c>
       <c r="D38" t="n">
-        <v>5.007953235628285</v>
+        <v>61.66107019199579</v>
       </c>
       <c r="E38" t="n">
-        <v>5.244192621134316</v>
+        <v>64.50513605302351</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.06167808181044032</v>
+        <v>-0.3198487744890628</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.9299792402237905</v>
+        <v>0.6310905068209727</v>
       </c>
       <c r="D39" t="n">
-        <v>-5.576527153801635</v>
+        <v>-13.8640558831852</v>
       </c>
       <c r="E39" t="n">
-        <v>-7.793051607713017</v>
+        <v>-40.54860518473068</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5614569134839866</v>
+        <v>0.6982831435042827</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.8934003961117531</v>
+        <v>-0.3324374603350742</v>
       </c>
       <c r="D40" t="n">
-        <v>-2.875629260017932</v>
+        <v>53.63111825001554</v>
       </c>
       <c r="E40" t="n">
-        <v>-4.377900903012026</v>
+        <v>35.54539776493383</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.4933161491432858</v>
+        <v>-0.9180926636496711</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.5454499185345714</v>
+        <v>-0.2897377752139949</v>
       </c>
       <c r="D41" t="n">
-        <v>1.731931059493485</v>
+        <v>85.27089028094365</v>
       </c>
       <c r="E41" t="n">
-        <v>1.954594934404862</v>
+        <v>87.95152172503208</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.8324883562683414</v>
+        <v>0.1699920405943107</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.5332165369331476</v>
+        <v>0.5555537882336548</v>
       </c>
       <c r="D42" t="n">
-        <v>5.011274283556021</v>
+        <v>-14.65652740682361</v>
       </c>
       <c r="E42" t="n">
-        <v>5.846531816449119</v>
+        <v>-4.600933038513421</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.3299122523917237</v>
+        <v>0.4041597782952169</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.6269844305098482</v>
+        <v>-0.3875075512776087</v>
       </c>
       <c r="D43" t="n">
-        <v>-1.080300613409902</v>
+        <v>22.93814754751341</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.8864710595203338</v>
+        <v>25.27164505426798</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.5125016184881652</v>
+        <v>0.2537010650709</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.8693023313266497</v>
+        <v>-0.468948937146175</v>
       </c>
       <c r="D44" t="n">
-        <v>-1.219004118526207</v>
+        <v>17.32256419462555</v>
       </c>
       <c r="E44" t="n">
-        <v>-1.349810442939055</v>
+        <v>15.74779798503599</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.4562622404139616</v>
+        <v>0.9585353857689112</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6388742054740928</v>
+        <v>0.7895226908564392</v>
       </c>
       <c r="D45" t="n">
-        <v>4.599595707382056</v>
+        <v>39.05529980704189</v>
       </c>
       <c r="E45" t="n">
-        <v>4.259026294038439</v>
+        <v>34.9552136180855</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.04638371212631975</v>
+        <v>-0.7840987078567054</v>
       </c>
       <c r="C46" t="n">
-        <v>0.05102603886394363</v>
+        <v>-0.9692357931475899</v>
       </c>
       <c r="D46" t="n">
-        <v>0.01817514597978535</v>
+        <v>148.5576194857422</v>
       </c>
       <c r="E46" t="n">
-        <v>-1.654136998477944</v>
+        <v>128.4247958719046</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.2452970443332452</v>
+        <v>0.422118265233453</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0419972644457729</v>
+        <v>-0.09946864989063409</v>
       </c>
       <c r="D47" t="n">
-        <v>0.6515579548121512</v>
+        <v>18.1590000202473</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.1626363687480108</v>
+        <v>8.35698383687509</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3903293580024056</v>
+        <v>-0.8418073506537791</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2741915455747761</v>
+        <v>0.6313519171369162</v>
       </c>
       <c r="D48" t="n">
-        <v>1.948370156599979</v>
+        <v>48.33428098950842</v>
       </c>
       <c r="E48" t="n">
-        <v>1.427355375688469</v>
+        <v>42.06182837409371</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.9859017774955614</v>
+        <v>-0.3765417863639733</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.2910116309888502</v>
+        <v>-0.621714024037993</v>
       </c>
       <c r="D49" t="n">
-        <v>9.043178513586357</v>
+        <v>36.93904776168671</v>
       </c>
       <c r="E49" t="n">
-        <v>10.23885794791304</v>
+        <v>51.33373073386471</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.4789146635581092</v>
+        <v>0.8688594508241474</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8512696276024665</v>
+        <v>-0.4061704248000999</v>
       </c>
       <c r="D50" t="n">
-        <v>5.833624244021098</v>
+        <v>84.003241273244</v>
       </c>
       <c r="E50" t="n">
-        <v>6.222280647136433</v>
+        <v>88.68224264044802</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.442693832403426</v>
+        <v>-0.4932144967980312</v>
       </c>
       <c r="C51" t="n">
-        <v>0.4737219774513339</v>
+        <v>0.3015515726431124</v>
       </c>
       <c r="D51" t="n">
-        <v>2.287617483984073</v>
+        <v>22.30842622968098</v>
       </c>
       <c r="E51" t="n">
-        <v>0.2934953253768504</v>
+        <v>-1.698640762410143</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.2853156761554017</v>
+        <v>0.6426343547078419</v>
       </c>
       <c r="C52" t="n">
-        <v>0.3207390593974342</v>
+        <v>-0.2395402088796597</v>
       </c>
       <c r="D52" t="n">
-        <v>1.288648534035373</v>
+        <v>43.4823546585462</v>
       </c>
       <c r="E52" t="n">
-        <v>1.655210249974612</v>
+        <v>47.89535996682456</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.3794695885724375</v>
+        <v>0.1425114941692878</v>
       </c>
       <c r="C53" t="n">
-        <v>0.4998203120818865</v>
+        <v>0.1840533448652848</v>
       </c>
       <c r="D53" t="n">
-        <v>1.946730519903219</v>
+        <v>1.308968124797571</v>
       </c>
       <c r="E53" t="n">
-        <v>1.511175432896601</v>
+        <v>-3.934642507269793</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.5969955897002779</v>
+        <v>-0.6829097946332319</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.2509440905329223</v>
+        <v>-0.3072831306137693</v>
       </c>
       <c r="D54" t="n">
-        <v>3.668249599735322</v>
+        <v>48.38978328840906</v>
       </c>
       <c r="E54" t="n">
-        <v>2.902603306114113</v>
+        <v>39.17223270662895</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.02303638816221021</v>
+        <v>0.06304872314011178</v>
       </c>
       <c r="C55" t="n">
-        <v>0.005727854690717349</v>
+        <v>-0.7586493264734526</v>
       </c>
       <c r="D55" t="n">
-        <v>0.008448389697878651</v>
+        <v>44.23108443499311</v>
       </c>
       <c r="E55" t="n">
-        <v>0.7002972042367906</v>
+        <v>52.5601934453634</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.3825845250099931</v>
+        <v>0.1947962041341214</v>
       </c>
       <c r="C56" t="n">
-        <v>0.2241663919120507</v>
+        <v>-0.8988514188923586</v>
       </c>
       <c r="D56" t="n">
-        <v>1.355193614076288</v>
+        <v>77.22086564916373</v>
       </c>
       <c r="E56" t="n">
-        <v>2.521326437012273</v>
+        <v>91.25983948086403</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.6398992139946655</v>
+        <v>0.6570936202374105</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7239605939605747</v>
+        <v>0.7881295738701457</v>
       </c>
       <c r="D57" t="n">
-        <v>5.832682770535864</v>
+        <v>-8.222178283867088</v>
       </c>
       <c r="E57" t="n">
-        <v>6.886025949221378</v>
+        <v>4.45893061771962</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.02245435673427076</v>
+        <v>0.04214139058416522</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.4090263866980317</v>
+        <v>-0.9814881196756289</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.5310022732723614</v>
+        <v>94.83906981168842</v>
       </c>
       <c r="E58" t="n">
-        <v>-1.480216194384341</v>
+        <v>83.41156418190455</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.7709437818589016</v>
+        <v>0.06292808658022109</v>
       </c>
       <c r="C59" t="n">
-        <v>0.2046833202650513</v>
+        <v>0.9958969977668954</v>
       </c>
       <c r="D59" t="n">
-        <v>6.416731352824671</v>
+        <v>-98.58561535701753</v>
       </c>
       <c r="E59" t="n">
-        <v>6.06699045297907</v>
+        <v>-102.7961162915901</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.01648717495557883</v>
+        <v>-0.5165682659594975</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.008535681113036597</v>
+        <v>-0.9240181228947502</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0004930890693058833</v>
+        <v>103.0471708622808</v>
       </c>
       <c r="E60" t="n">
-        <v>0.375175280446961</v>
+        <v>107.5579378834092</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.4341100716521393</v>
+        <v>-0.7764778809834336</v>
       </c>
       <c r="C61" t="n">
-        <v>0.5996639989701711</v>
+        <v>0.4902207702760648</v>
       </c>
       <c r="D61" t="n">
-        <v>2.889891827157039</v>
+        <v>50.38558293040208</v>
       </c>
       <c r="E61" t="n">
-        <v>3.993301836735495</v>
+        <v>63.66944214903458</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.790239389326461</v>
+        <v>-0.8502289585388028</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.6790142690955754</v>
+        <v>-0.1712193412313048</v>
       </c>
       <c r="D62" t="n">
-        <v>2.991271766442376</v>
+        <v>71.96085284914793</v>
       </c>
       <c r="E62" t="n">
-        <v>2.449292071530421</v>
+        <v>65.43600541793937</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-5.019450631205125e-05</v>
+        <v>-0.3042022032960088</v>
       </c>
       <c r="C63" t="n">
-        <v>0.5168177912309293</v>
+        <v>0.07354504957184793</v>
       </c>
       <c r="D63" t="n">
-        <v>1.01792140305682</v>
+        <v>9.302915571274884</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8079280695621055</v>
+        <v>6.774823697193709</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.08551266788755041</v>
+        <v>-0.009950805174019806</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.878264967499401</v>
+        <v>-0.6291279088254351</v>
       </c>
       <c r="D64" t="n">
-        <v>-4.615191840823298</v>
+        <v>24.81569611485833</v>
       </c>
       <c r="E64" t="n">
-        <v>-5.866534347003291</v>
+        <v>9.750890156884221</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.9082000566132071</v>
+        <v>-0.9833382283832373</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.767857647085354</v>
+        <v>-0.3783423413227713</v>
       </c>
       <c r="D65" t="n">
-        <v>3.698440027840316</v>
+        <v>100.114749668311</v>
       </c>
       <c r="E65" t="n">
-        <v>2.345446377584387</v>
+        <v>83.82617423607451</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.0853154548894528</v>
+        <v>0.6479831944795984</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.4960643257333781</v>
+        <v>-0.695958633561313</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.7552067258768602</v>
+        <v>77.94761436975278</v>
       </c>
       <c r="E66" t="n">
-        <v>0.163817008181804</v>
+        <v>89.01166290641707</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.8919100405540348</v>
+        <v>-0.4855566405546299</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.0693983783984109</v>
+        <v>-0.2454204518165735</v>
       </c>
       <c r="D67" t="n">
-        <v>7.911152525965866</v>
+        <v>24.38579654572525</v>
       </c>
       <c r="E67" t="n">
-        <v>9.445155189000353</v>
+        <v>42.85352408115195</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.2343004083501838</v>
+        <v>-0.6130735616543666</v>
       </c>
       <c r="C68" t="n">
-        <v>0.5469373059077962</v>
+        <v>-0.1004527180968482</v>
       </c>
       <c r="D68" t="n">
-        <v>1.469212609833273</v>
+        <v>37.30800635585386</v>
       </c>
       <c r="E68" t="n">
-        <v>1.387764108135477</v>
+        <v>36.3274547741844</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.6531702354534958</v>
+        <v>0.3508849177611184</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7136308562528624</v>
+        <v>0.7783374612396814</v>
       </c>
       <c r="D69" t="n">
-        <v>5.884125260809406</v>
+        <v>-36.09298934142006</v>
       </c>
       <c r="E69" t="n">
-        <v>7.019191403512252</v>
+        <v>-22.42802462965239</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.008184855241341937</v>
+        <v>-0.6050826344410729</v>
       </c>
       <c r="C70" t="n">
-        <v>0.8056725469705073</v>
+        <v>0.5954913193746263</v>
       </c>
       <c r="D70" t="n">
-        <v>3.728010957239567</v>
+        <v>17.29643519697847</v>
       </c>
       <c r="E70" t="n">
-        <v>4.137046683796659</v>
+        <v>22.22078150506688</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.1586201901567554</v>
+        <v>-0.7937274871341833</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1403083560679679</v>
+        <v>-0.604922686512712</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2245961867128068</v>
+        <v>82.59577253058087</v>
       </c>
       <c r="E71" t="n">
-        <v>-0.5050795349094578</v>
+        <v>73.81126860444077</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.9798303335318344</v>
+        <v>0.9318892782214903</v>
       </c>
       <c r="C72" t="n">
-        <v>0.2845541581939639</v>
+        <v>-0.2189184012317049</v>
       </c>
       <c r="D72" t="n">
-        <v>9.134802196628064</v>
+        <v>88.98227059852407</v>
       </c>
       <c r="E72" t="n">
-        <v>9.543565991811917</v>
+        <v>93.90334314794809</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.830351451134915</v>
+        <v>0.391921342757152</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.1291338350183866</v>
+        <v>0.3863244750531558</v>
       </c>
       <c r="D73" t="n">
-        <v>6.735430509374736</v>
+        <v>8.915252996807638</v>
       </c>
       <c r="E73" t="n">
-        <v>8.475057816562721</v>
+        <v>29.85847812705858</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.4487369574505953</v>
+        <v>0.9000265212931671</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.4739534750091063</v>
+        <v>0.6292665641489459</v>
       </c>
       <c r="D74" t="n">
-        <v>0.8405105618473387</v>
+        <v>53.40844880598547</v>
       </c>
       <c r="E74" t="n">
-        <v>0.799988797083799</v>
+        <v>52.92061072790328</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.06387243330467873</v>
+        <v>-0.6600296796615552</v>
       </c>
       <c r="C75" t="n">
-        <v>0.6959837400658753</v>
+        <v>0.4780479217095994</v>
       </c>
       <c r="D75" t="n">
-        <v>2.375009005848729</v>
+        <v>34.19852837826608</v>
       </c>
       <c r="E75" t="n">
-        <v>4.144730798567048</v>
+        <v>55.50405845914446</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.6359475884248171</v>
+        <v>-0.7569814979665623</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1729858134349052</v>
+        <v>-0.1348787347145435</v>
       </c>
       <c r="D76" t="n">
-        <v>3.81421245631046</v>
+        <v>56.94778434729856</v>
       </c>
       <c r="E76" t="n">
-        <v>0.8510968709519848</v>
+        <v>21.27508794002613</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.9816503712409568</v>
+        <v>0.5423242241084059</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.6818373278733265</v>
+        <v>-0.07977176462247981</v>
       </c>
       <c r="D77" t="n">
-        <v>8.589764037682631</v>
+        <v>29.72488549027981</v>
       </c>
       <c r="E77" t="n">
-        <v>9.519393457185101</v>
+        <v>40.9166149715881</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.005818402290541869</v>
+        <v>-0.1584543565213645</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.2268987264580853</v>
+        <v>-0.4385306621296161</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.1061799113775859</v>
+        <v>10.53698985994515</v>
       </c>
       <c r="E78" t="n">
-        <v>-0.007723567608252518</v>
+        <v>11.72229740515472</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.3714233640354083</v>
+        <v>-0.791360483413585</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.01098126124406629</v>
+        <v>0.04622812293114253</v>
       </c>
       <c r="D79" t="n">
-        <v>1.407430700341795</v>
+        <v>62.72366465158368</v>
       </c>
       <c r="E79" t="n">
-        <v>1.06923240046941</v>
+        <v>58.65212409595472</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.2727511091622636</v>
+        <v>-0.3040918929059917</v>
       </c>
       <c r="C80" t="n">
-        <v>0.04483500767949589</v>
+        <v>0.461986808143529</v>
       </c>
       <c r="D80" t="n">
-        <v>0.8007787677197491</v>
+        <v>0.1051415322326155</v>
       </c>
       <c r="E80" t="n">
-        <v>0.9045666464154578</v>
+        <v>1.354634972772472</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.08111021555299858</v>
+        <v>0.8709492337189941</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.9389552859882375</v>
+        <v>-0.295777627977573</v>
       </c>
       <c r="D81" t="n">
-        <v>-5.678624389679264</v>
+        <v>79.78840341020046</v>
       </c>
       <c r="E81" t="n">
-        <v>-7.926704334034866</v>
+        <v>52.7239602441829</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.1427156067511872</v>
+        <v>0.04500460018204366</v>
       </c>
       <c r="C82" t="n">
-        <v>0.439998439272447</v>
+        <v>0.873946197196295</v>
       </c>
       <c r="D82" t="n">
-        <v>0.9838197918952118</v>
+        <v>-66.65265507027559</v>
       </c>
       <c r="E82" t="n">
-        <v>0.7353554685912786</v>
+        <v>-69.64389591725973</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.4793182136338827</v>
+        <v>0.7649911199517176</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3536845252602541</v>
+        <v>0.9901788442878243</v>
       </c>
       <c r="D83" t="n">
-        <v>3.029518215738307</v>
+        <v>-42.17322684444788</v>
       </c>
       <c r="E83" t="n">
-        <v>3.433437598857669</v>
+        <v>-37.31047575966812</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.9969029160968941</v>
+        <v>0.4399546182659235</v>
       </c>
       <c r="C84" t="n">
-        <v>0.6255708438592831</v>
+        <v>-0.4666705362188657</v>
       </c>
       <c r="D84" t="n">
-        <v>13.06133977094095</v>
+        <v>30.5431200854497</v>
       </c>
       <c r="E84" t="n">
-        <v>14.73294166482201</v>
+        <v>50.66739305302843</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.08708884175221732</v>
+        <v>0.3609964991533388</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.3540058096164784</v>
+        <v>-0.1779432481848331</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.2171532267401139</v>
+        <v>13.93477294802423</v>
       </c>
       <c r="E85" t="n">
-        <v>-0.8033532195548253</v>
+        <v>6.877561112970335</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.5004128935183039</v>
+        <v>-0.2891999331675694</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.7603139795761495</v>
+        <v>0.2950525656756422</v>
       </c>
       <c r="D86" t="n">
-        <v>-1.359443325887403</v>
+        <v>6.222281206104896</v>
       </c>
       <c r="E86" t="n">
-        <v>-2.273906336680136</v>
+        <v>-4.786861171222569</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.4275268192483859</v>
+        <v>-0.09355813547180958</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.7594320984457046</v>
+        <v>-0.8422753607540172</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.7074976283550021</v>
+        <v>60.14107477374224</v>
       </c>
       <c r="E87" t="n">
-        <v>-1.27502006158246</v>
+        <v>53.30872048932764</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.8689447674681618</v>
+        <v>0.9329830310124321</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.6162873730613621</v>
+        <v>0.4637396574672501</v>
       </c>
       <c r="D88" t="n">
-        <v>4.866371157843714</v>
+        <v>75.04917110725376</v>
       </c>
       <c r="E88" t="n">
-        <v>5.901755202497033</v>
+        <v>87.51407152232929</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.8768918058528758</v>
+        <v>-0.3941952911831141</v>
       </c>
       <c r="C89" t="n">
-        <v>0.5672282689567938</v>
+        <v>-0.3054126440847185</v>
       </c>
       <c r="D89" t="n">
-        <v>10.10613160804239</v>
+        <v>17.71586478673328</v>
       </c>
       <c r="E89" t="n">
-        <v>10.47797218719483</v>
+        <v>22.19242188006877</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.4832469272882356</v>
+        <v>0.01654486372373842</v>
       </c>
       <c r="C90" t="n">
-        <v>0.702902249541733</v>
+        <v>0.8391369335525727</v>
       </c>
       <c r="D90" t="n">
-        <v>5.56422968734362</v>
+        <v>-59.0443693405753</v>
       </c>
       <c r="E90" t="n">
-        <v>4.965033714485713</v>
+        <v>-66.25803867357044</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-0.4251971581236265</v>
+        <v>-0.3238667439270566</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.3648456619531026</v>
+        <v>-0.3786465837140276</v>
       </c>
       <c r="D91" t="n">
-        <v>1.699226365844701</v>
+        <v>15.23433884503934</v>
       </c>
       <c r="E91" t="n">
-        <v>2.279767857511527</v>
+        <v>22.22342846624301</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.05043595275522295</v>
+        <v>0.2431772339480642</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.7452970013161559</v>
+        <v>0.8761038239265071</v>
       </c>
       <c r="D92" t="n">
-        <v>-3.017146241737718</v>
+        <v>-62.28583973568669</v>
       </c>
       <c r="E92" t="n">
-        <v>-2.907344719821511</v>
+        <v>-60.96394855610267</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.3796988753079562</v>
+        <v>0.4548367065342196</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8019949572771687</v>
+        <v>-0.5806123654997133</v>
       </c>
       <c r="D93" t="n">
-        <v>5.779794051860228</v>
+        <v>41.56854967339385</v>
       </c>
       <c r="E93" t="n">
-        <v>6.87539952265457</v>
+        <v>54.7584507136751</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.160349168749178</v>
+        <v>-0.1222383483077731</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4263802258935261</v>
+        <v>0.4561273334926217</v>
       </c>
       <c r="D94" t="n">
-        <v>0.6895940003965425</v>
+        <v>-7.683435445852775</v>
       </c>
       <c r="E94" t="n">
-        <v>-0.1044773239355733</v>
+        <v>-17.2431925537394</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.3302712791928246</v>
+        <v>0.03437538510046245</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9527075822396023</v>
+        <v>0.0511286610605195</v>
       </c>
       <c r="D95" t="n">
-        <v>6.576817749958067</v>
+        <v>0.1045635299188433</v>
       </c>
       <c r="E95" t="n">
-        <v>6.206208864459946</v>
+        <v>-4.357165308314329</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.7134113439807968</v>
+        <v>0.6001507220594138</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.6124596480862541</v>
+        <v>-0.9336152572300882</v>
       </c>
       <c r="D96" t="n">
-        <v>4.222677140255817</v>
+        <v>120.1636938914213</v>
       </c>
       <c r="E96" t="n">
-        <v>3.77917529808109</v>
+        <v>114.8244129500566</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.6750039375280479</v>
+        <v>-0.566632787669749</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.3982867363297973</v>
+        <v>-0.7461801275835085</v>
       </c>
       <c r="D97" t="n">
-        <v>3.604016591173855</v>
+        <v>71.40811371239809</v>
       </c>
       <c r="E97" t="n">
-        <v>1.948678464786875</v>
+        <v>51.47963885783314</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.9084212572536554</v>
+        <v>0.2767430925056189</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.4534948211072669</v>
+        <v>-0.5783849106991907</v>
       </c>
       <c r="D98" t="n">
-        <v>6.821003333098134</v>
+        <v>27.77748853516974</v>
       </c>
       <c r="E98" t="n">
-        <v>7.155936150317995</v>
+        <v>31.80971622299755</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.2192381915177724</v>
+        <v>0.5763915516529643</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9907954148719071</v>
+        <v>-0.490263310877219</v>
       </c>
       <c r="D99" t="n">
-        <v>7.844575062155222</v>
+        <v>46.42812953435049</v>
       </c>
       <c r="E99" t="n">
-        <v>8.139846897735197</v>
+        <v>49.98288203887967</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.655308769228488</v>
+        <v>-0.9863141487899358</v>
       </c>
       <c r="C100" t="n">
-        <v>0.4329103861408079</v>
+        <v>0.07059867520371355</v>
       </c>
       <c r="D100" t="n">
-        <v>4.272602445460303</v>
+        <v>97.5029632235005</v>
       </c>
       <c r="E100" t="n">
-        <v>4.278386123822247</v>
+        <v>97.57259243517971</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-0.6612794202262902</v>
+        <v>0.9414831245644188</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.2246659564347393</v>
+        <v>0.2272024584014094</v>
       </c>
       <c r="D101" t="n">
-        <v>4.502064353400205</v>
+        <v>86.51353870413413</v>
       </c>
       <c r="E101" t="n">
-        <v>4.236729840533546</v>
+        <v>83.31919908045093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring and saved report
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.7883267274870609</v>
+        <v>0.6601716109879077</v>
       </c>
       <c r="C2" t="n">
-        <v>0.800085954409169</v>
+        <v>-0.7420253700032422</v>
       </c>
       <c r="D2" t="n">
-        <v>14.08421954069435</v>
+        <v>4.270818430237561</v>
       </c>
       <c r="E2" t="n">
-        <v>20.84790550155498</v>
+        <v>4.986300808699939</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4067218946723166</v>
+        <v>-0.6577905566668394</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.8024105160763451</v>
+        <v>0.5416984996851222</v>
       </c>
       <c r="D3" t="n">
-        <v>69.79870575383211</v>
+        <v>1.064648331030498</v>
       </c>
       <c r="E3" t="n">
-        <v>67.91598043374525</v>
+        <v>0.86548816927815</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3217520894772643</v>
+        <v>0.09007713176002641</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7404537878180328</v>
+        <v>-0.2608401713425628</v>
       </c>
       <c r="D4" t="n">
-        <v>52.09877729250569</v>
+        <v>0.04731675134610744</v>
       </c>
       <c r="E4" t="n">
-        <v>60.91825997807945</v>
+        <v>0.9802672882570709</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6570128138945719</v>
+        <v>0.8907905122855158</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2581283720985377</v>
+        <v>0.2190924993833352</v>
       </c>
       <c r="D5" t="n">
-        <v>40.69021367644633</v>
+        <v>9.143441371550756</v>
       </c>
       <c r="E5" t="n">
-        <v>61.42909457063656</v>
+        <v>11.33726052795274</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2977538290088548</v>
+        <v>-0.7370357249236463</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3968395867426517</v>
+        <v>-0.6242445150629783</v>
       </c>
       <c r="D6" t="n">
-        <v>3.216949784596996</v>
+        <v>9.75942615207256</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02851659077062552</v>
+        <v>9.422144412753454</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8379969398586182</v>
+        <v>-0.4362235442361808</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6350416081076644</v>
+        <v>0.4328403625239201</v>
       </c>
       <c r="D7" t="n">
-        <v>47.25458515088006</v>
+        <v>0.2020296901037268</v>
       </c>
       <c r="E7" t="n">
-        <v>44.06637551554883</v>
+        <v>-0.135228400547366</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.745702201662465</v>
+        <v>-0.1375577118130988</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9992229584316992</v>
+        <v>-0.4926364210269423</v>
       </c>
       <c r="D8" t="n">
-        <v>-47.71101254850895</v>
+        <v>1.369705210103058</v>
       </c>
       <c r="E8" t="n">
-        <v>-26.2070962926398</v>
+        <v>3.644452032773008</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.7525429745663264</v>
+        <v>0.3481886954441162</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8592508216668169</v>
+        <v>-0.9273787197211165</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.563637588771424</v>
+        <v>4.800040969438167</v>
       </c>
       <c r="E9" t="n">
-        <v>6.886411945716119</v>
+        <v>5.905477611418725</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.9036575038632009</v>
+        <v>-0.6818438902964727</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1333062515789742</v>
+        <v>-0.299516659401097</v>
       </c>
       <c r="D10" t="n">
-        <v>81.94807664600607</v>
+        <v>5.964404435176313</v>
       </c>
       <c r="E10" t="n">
-        <v>75.55531071839602</v>
+        <v>5.288159056945047</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.5874227318484027</v>
+        <v>0.4670435387166465</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7630646847948557</v>
+        <v>0.1593041632113614</v>
       </c>
       <c r="D11" t="n">
-        <v>-7.665474409358794</v>
+        <v>2.662043778815145</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.2775114784065682</v>
+        <v>3.44356399137643</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.3067545647977408</v>
+        <v>-0.4513216717555475</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.004970795907636161</v>
+        <v>0.831354081445655</v>
       </c>
       <c r="D12" t="n">
-        <v>9.371051976924006</v>
+        <v>-4.198463265009589</v>
       </c>
       <c r="E12" t="n">
-        <v>3.06075917796043</v>
+        <v>-4.865984395754397</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5644116894058673</v>
+        <v>-0.7291312781870849</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8041349689470894</v>
+        <v>0.01938648805631349</v>
       </c>
       <c r="D13" t="n">
-        <v>-22.27443032219932</v>
+        <v>5.160486957427988</v>
       </c>
       <c r="E13" t="n">
-        <v>-28.61620612359669</v>
+        <v>4.489635463092554</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.8997496845279418</v>
+        <v>-0.6847274588092451</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5039019772166953</v>
+        <v>0.1278197177025777</v>
       </c>
       <c r="D14" t="n">
-        <v>70.38735488914189</v>
+        <v>4.093078008758599</v>
       </c>
       <c r="E14" t="n">
-        <v>73.68212072041089</v>
+        <v>4.441607923818843</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.8430710240680073</v>
+        <v>0.7618079982642816</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9810635957087623</v>
+        <v>0.5964488099618972</v>
       </c>
       <c r="D15" t="n">
-        <v>-19.1997700282388</v>
+        <v>7.180305199118632</v>
       </c>
       <c r="E15" t="n">
-        <v>-45.25263494366892</v>
+        <v>4.424357353030411</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8514766189779066</v>
+        <v>-0.2418956531068208</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08345352652200022</v>
+        <v>-0.8666966550256991</v>
       </c>
       <c r="D16" t="n">
-        <v>72.18132151395056</v>
+        <v>6.289390533075492</v>
       </c>
       <c r="E16" t="n">
-        <v>48.69336076896509</v>
+        <v>3.804765712186434</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5129950434980493</v>
+        <v>-0.1308035214710739</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.2376006257412293</v>
+        <v>0.6011866037649236</v>
       </c>
       <c r="D17" t="n">
-        <v>28.29472255908012</v>
+        <v>-1.774678505797663</v>
       </c>
       <c r="E17" t="n">
-        <v>20.6381332623218</v>
+        <v>-2.584614796845861</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.9895408966379746</v>
+        <v>-0.9242029828355653</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9365270184260108</v>
+        <v>0.3008350840794192</v>
       </c>
       <c r="D18" t="n">
-        <v>20.4062969249014</v>
+        <v>6.620395946270467</v>
       </c>
       <c r="E18" t="n">
-        <v>6.61471964086584</v>
+        <v>5.161482777470138</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7831680939175434</v>
+        <v>0.5606838444768714</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6101219877323796</v>
+        <v>0.4976054088161337</v>
       </c>
       <c r="D19" t="n">
-        <v>36.37369475628973</v>
+        <v>4.061000033915709</v>
       </c>
       <c r="E19" t="n">
-        <v>40.65275598059209</v>
+        <v>4.513651579251563</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.199814456183109</v>
+        <v>0.02531840070295654</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.3380624954873288</v>
+        <v>0.08081077221387201</v>
       </c>
       <c r="D20" t="n">
-        <v>8.180095270900543</v>
+        <v>0.02560505263845424</v>
       </c>
       <c r="E20" t="n">
-        <v>-4.184339393370797</v>
+        <v>-1.282340817871755</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3198043211807147</v>
+        <v>-0.1743071937027494</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.003899044295286869</v>
+        <v>0.9578099850724975</v>
       </c>
       <c r="D21" t="n">
-        <v>10.18888131950782</v>
+        <v>-6.770402710955988</v>
       </c>
       <c r="E21" t="n">
-        <v>-9.042257272544731</v>
+        <v>-8.804728500178554</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.01526721880575921</v>
+        <v>0.3768619685565402</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.9229619526462962</v>
+        <v>0.4946252636686568</v>
       </c>
       <c r="D22" t="n">
-        <v>78.62631764166164</v>
+        <v>1.77874599083716</v>
       </c>
       <c r="E22" t="n">
-        <v>98.583848430367</v>
+        <v>3.889911659907063</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.600864302517591</v>
+        <v>0.2514135864542379</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.6901452826030117</v>
+        <v>0.2236662913566698</v>
       </c>
       <c r="D23" t="n">
-        <v>71.03993630897288</v>
+        <v>0.9386675050707869</v>
       </c>
       <c r="E23" t="n">
-        <v>67.96557254333784</v>
+        <v>0.613452361726784</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.7070253064025853</v>
+        <v>-0.8995594822143487</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5862124932915631</v>
+        <v>0.1885740108469549</v>
       </c>
       <c r="D24" t="n">
-        <v>27.90056248807203</v>
+        <v>6.956232785170121</v>
       </c>
       <c r="E24" t="n">
-        <v>28.82008444499824</v>
+        <v>7.053502492929621</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.5659865789389336</v>
+        <v>0.9801210197461934</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.2908965280207036</v>
+        <v>-0.5710663792579485</v>
       </c>
       <c r="D25" t="n">
-        <v>33.58676419096425</v>
+        <v>7.592633045034922</v>
       </c>
       <c r="E25" t="n">
-        <v>14.1861708186315</v>
+        <v>5.540381836161252</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1704155445933895</v>
+        <v>-0.8182890617882983</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.5668478282546454</v>
+        <v>-0.7034301704556347</v>
       </c>
       <c r="D26" t="n">
-        <v>21.56125473815938</v>
+        <v>12.43392294621905</v>
       </c>
       <c r="E26" t="n">
-        <v>14.14847262014558</v>
+        <v>11.64977728784418</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.137885576416714</v>
+        <v>-0.4588297104026542</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.3505592017192578</v>
+        <v>0.9636195364071038</v>
       </c>
       <c r="D27" t="n">
-        <v>6.429744658691332</v>
+        <v>-6.760565131675304</v>
       </c>
       <c r="E27" t="n">
-        <v>7.940161783338793</v>
+        <v>-6.600788813988969</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.7598851424733513</v>
+        <v>-0.9832528886575727</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.7837352789227821</v>
+        <v>-0.9748654519819226</v>
       </c>
       <c r="D28" t="n">
-        <v>108.85813509274</v>
+        <v>21.70861622349479</v>
       </c>
       <c r="E28" t="n">
-        <v>93.18521928501201</v>
+        <v>20.05068959229931</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.006121628562932635</v>
+        <v>-0.4306572050387396</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8085434330345842</v>
+        <v>0.7948808672313372</v>
       </c>
       <c r="D29" t="n">
-        <v>52.80617242694299</v>
+        <v>-3.678486556270155</v>
       </c>
       <c r="E29" t="n">
-        <v>57.92199889736433</v>
+        <v>-3.137319548807243</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.5778692615891516</v>
+        <v>-0.4041124666284004</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.5221182061656144</v>
+        <v>0.2497580995677757</v>
       </c>
       <c r="D30" t="n">
-        <v>46.00803906582677</v>
+        <v>0.9029934372866339</v>
       </c>
       <c r="E30" t="n">
-        <v>37.82922746981076</v>
+        <v>0.03781495212695096</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.7461202387056165</v>
+        <v>0.2182710659628795</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2742859745515567</v>
+        <v>-0.3316322201827497</v>
       </c>
       <c r="D31" t="n">
-        <v>52.68480002550503</v>
+        <v>0.2860823749864661</v>
       </c>
       <c r="E31" t="n">
-        <v>48.71284772982933</v>
+        <v>-0.1340822944103889</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.5372641962823503</v>
+        <v>-0.1712046574421786</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2251356548244388</v>
+        <v>0.1829034479921863</v>
       </c>
       <c r="D32" t="n">
-        <v>27.19561101253748</v>
+        <v>0.06356515061768697</v>
       </c>
       <c r="E32" t="n">
-        <v>19.00225767033677</v>
+        <v>-0.803151602759568</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.8949254046015516</v>
+        <v>0.02275272003121853</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.08774207566073966</v>
+        <v>0.5770044125204641</v>
       </c>
       <c r="D33" t="n">
-        <v>79.66581791401077</v>
+        <v>-1.200807986339967</v>
       </c>
       <c r="E33" t="n">
-        <v>104.8880264543183</v>
+        <v>1.467270611767667</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.05914426922634908</v>
+        <v>-0.119520545724797</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.1792469726263153</v>
+        <v>-0.9286237774343524</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9667124958665121</v>
+        <v>6.309514678612412</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7829227066746588</v>
+        <v>6.29007286001394</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.3202157862062349</v>
+        <v>0.2879249668266051</v>
       </c>
       <c r="C35" t="n">
-        <v>0.6992849473576421</v>
+        <v>-0.2745917802742632</v>
       </c>
       <c r="D35" t="n">
-        <v>-22.7836623123874</v>
+        <v>0.5009009914554854</v>
       </c>
       <c r="E35" t="n">
-        <v>-37.18636156598828</v>
+        <v>-1.022658437216371</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.3451356101837937</v>
+        <v>-0.1848039521941576</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.7701527628759548</v>
+        <v>0.5232229387771894</v>
       </c>
       <c r="D36" t="n">
-        <v>56.15177170947156</v>
+        <v>-1.207465895251709</v>
       </c>
       <c r="E36" t="n">
-        <v>67.35224876542505</v>
+        <v>-0.02264684683935458</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.02303954825946541</v>
+        <v>0.5381055630462426</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.1628023249015498</v>
+        <v>0.9807847761350361</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4472444320869069</v>
+        <v>-0.3901248881962176</v>
       </c>
       <c r="E37" t="n">
-        <v>-16.17680987692755</v>
+        <v>-2.148665717195315</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.8379980196241088</v>
+        <v>0.8773721693415755</v>
       </c>
       <c r="C38" t="n">
-        <v>0.471818754638156</v>
+        <v>0.7930770240696394</v>
       </c>
       <c r="D38" t="n">
-        <v>61.66107019199579</v>
+        <v>8.548048344577069</v>
       </c>
       <c r="E38" t="n">
-        <v>64.50513605302351</v>
+        <v>8.848901905568365</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.3198487744890628</v>
+        <v>0.7915404683771203</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6310905068209727</v>
+        <v>-0.7753419972605025</v>
       </c>
       <c r="D39" t="n">
-        <v>-13.8640558831852</v>
+        <v>5.847401754949177</v>
       </c>
       <c r="E39" t="n">
-        <v>-40.54860518473068</v>
+        <v>3.024632496744735</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.6982831435042827</v>
+        <v>-0.8173839988124509</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.3324374603350742</v>
+        <v>-0.387482715173709</v>
       </c>
       <c r="D40" t="n">
-        <v>53.63111825001554</v>
+        <v>8.868256697581579</v>
       </c>
       <c r="E40" t="n">
-        <v>35.54539776493383</v>
+        <v>6.955096568067598</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.9180926636496711</v>
+        <v>0.2029175863657946</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.2897377752139949</v>
+        <v>-0.289940625987702</v>
       </c>
       <c r="D41" t="n">
-        <v>85.27089028094365</v>
+        <v>0.2206670135384639</v>
       </c>
       <c r="E41" t="n">
-        <v>87.95152172503208</v>
+        <v>0.504232006427842</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.1699920405943107</v>
+        <v>0.003568278720374574</v>
       </c>
       <c r="C42" t="n">
-        <v>0.5555537882336548</v>
+        <v>-0.5183479187364353</v>
       </c>
       <c r="D42" t="n">
-        <v>-14.65652740682361</v>
+        <v>0.912456297976264</v>
       </c>
       <c r="E42" t="n">
-        <v>-4.600933038513421</v>
+        <v>1.976166324894192</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.4041597782952169</v>
+        <v>0.5782020891481092</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.3875075512776087</v>
+        <v>0.2707970143937481</v>
       </c>
       <c r="D43" t="n">
-        <v>22.93814754751341</v>
+        <v>4.228524111407247</v>
       </c>
       <c r="E43" t="n">
-        <v>25.27164505426798</v>
+        <v>4.475368266492228</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.2537010650709</v>
+        <v>0.6310925033788195</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.468948937146175</v>
+        <v>-0.7930132509468328</v>
       </c>
       <c r="D44" t="n">
-        <v>17.32256419462555</v>
+        <v>4.454712888599015</v>
       </c>
       <c r="E44" t="n">
-        <v>15.74779798503599</v>
+        <v>4.288129537497368</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.9585353857689112</v>
+        <v>0.9470700010447128</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7895226908564392</v>
+        <v>-0.7042774474384761</v>
       </c>
       <c r="D45" t="n">
-        <v>39.05529980704189</v>
+        <v>7.436979308222686</v>
       </c>
       <c r="E45" t="n">
-        <v>34.9552136180855</v>
+        <v>7.003260262815972</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.7840987078567054</v>
+        <v>0.05258332140162891</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.9692357931475899</v>
+        <v>0.1475369495572014</v>
       </c>
       <c r="D46" t="n">
-        <v>148.5576194857422</v>
+        <v>0.07172976710108911</v>
       </c>
       <c r="E46" t="n">
-        <v>128.4247958719046</v>
+        <v>-2.05797888698893</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.422118265233453</v>
+        <v>0.8208058171760202</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.09946864989063409</v>
+        <v>0.9100892663500566</v>
       </c>
       <c r="D47" t="n">
-        <v>18.1590000202473</v>
+        <v>6.115801284233272</v>
       </c>
       <c r="E47" t="n">
-        <v>8.35698383687509</v>
+        <v>5.078915495450509</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.8418073506537791</v>
+        <v>-0.6143533084408594</v>
       </c>
       <c r="C48" t="n">
-        <v>0.6313519171369162</v>
+        <v>0.744224731851771</v>
       </c>
       <c r="D48" t="n">
-        <v>48.33428098950842</v>
+        <v>-1.841443156893109</v>
       </c>
       <c r="E48" t="n">
-        <v>42.06182837409371</v>
+        <v>-2.504961442934059</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.3765417863639733</v>
+        <v>0.579526041185098</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.621714024037993</v>
+        <v>0.09893055218341895</v>
       </c>
       <c r="D49" t="n">
-        <v>36.93904776168671</v>
+        <v>3.763569161802632</v>
       </c>
       <c r="E49" t="n">
-        <v>51.33373073386471</v>
+        <v>5.286280604903891</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.8688594508241474</v>
+        <v>-0.2882188581859915</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.4061704248000999</v>
+        <v>-0.4044455032943419</v>
       </c>
       <c r="D50" t="n">
-        <v>84.003241273244</v>
+        <v>1.923951103984979</v>
       </c>
       <c r="E50" t="n">
-        <v>88.68224264044802</v>
+        <v>2.418909481178747</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.4932144967980312</v>
+        <v>0.3475433568596666</v>
       </c>
       <c r="C51" t="n">
-        <v>0.3015515726431124</v>
+        <v>0.8375466603904462</v>
       </c>
       <c r="D51" t="n">
-        <v>22.30842622968098</v>
+        <v>-1.039805946626231</v>
       </c>
       <c r="E51" t="n">
-        <v>-1.698640762410143</v>
+        <v>-3.579343336564632</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.6426343547078419</v>
+        <v>-0.02171678191628401</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.2395402088796597</v>
+        <v>0.9390481360720671</v>
       </c>
       <c r="D52" t="n">
-        <v>43.4823546585462</v>
+        <v>-5.822352772885137</v>
       </c>
       <c r="E52" t="n">
-        <v>47.89535996682456</v>
+        <v>-5.355532232664144</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.1425114941692878</v>
+        <v>0.3214996916734061</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1840533448652848</v>
+        <v>0.4140725541779864</v>
       </c>
       <c r="D53" t="n">
-        <v>1.308968124797571</v>
+        <v>1.408956133855417</v>
       </c>
       <c r="E53" t="n">
-        <v>-3.934642507269793</v>
+        <v>0.8542717460124317</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.6829097946332319</v>
+        <v>0.1396449706657175</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.3072831306137693</v>
+        <v>0.2675229462784174</v>
       </c>
       <c r="D54" t="n">
-        <v>48.38978328840906</v>
+        <v>0.3258498119042283</v>
       </c>
       <c r="E54" t="n">
-        <v>39.17223270662895</v>
+        <v>-0.6492095051623128</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.06304872314011178</v>
+        <v>-0.3634220280899987</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.7586493264734526</v>
+        <v>0.1865768499600544</v>
       </c>
       <c r="D55" t="n">
-        <v>44.23108443499311</v>
+        <v>0.8507699801410415</v>
       </c>
       <c r="E55" t="n">
-        <v>52.5601934453634</v>
+        <v>1.731847363049855</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.1947962041341214</v>
+        <v>0.8366308697459344</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.8988514188923586</v>
+        <v>0.9072398542264835</v>
       </c>
       <c r="D56" t="n">
-        <v>77.22086564916373</v>
+        <v>6.500905174871431</v>
       </c>
       <c r="E56" t="n">
-        <v>91.25983948086403</v>
+        <v>7.985988670231985</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.6570936202374105</v>
+        <v>-0.014873089059388</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7881295738701457</v>
+        <v>-0.8711755234133918</v>
       </c>
       <c r="D57" t="n">
-        <v>-8.222178283867088</v>
+        <v>4.619580738381517</v>
       </c>
       <c r="E57" t="n">
-        <v>4.45893061771962</v>
+        <v>5.961025331012072</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.04214139058416522</v>
+        <v>-0.9687245970242016</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.9814881196756289</v>
+        <v>0.7015387762096723</v>
       </c>
       <c r="D58" t="n">
-        <v>94.83906981168842</v>
+        <v>2.863098817196008</v>
       </c>
       <c r="E58" t="n">
-        <v>83.41156418190455</v>
+        <v>1.654264025751962</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.06292808658022109</v>
+        <v>0.8481490587914116</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9958969977668954</v>
+        <v>-0.06535188174948203</v>
       </c>
       <c r="D59" t="n">
-        <v>-98.58561535701753</v>
+        <v>6.941232920043901</v>
       </c>
       <c r="E59" t="n">
-        <v>-102.7961162915901</v>
+        <v>6.495833881617414</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.5165682659594975</v>
+        <v>-0.9488575920651898</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.9240181228947502</v>
+        <v>-0.5250434561016888</v>
       </c>
       <c r="D60" t="n">
-        <v>103.0471708622808</v>
+        <v>12.85823943746735</v>
       </c>
       <c r="E60" t="n">
-        <v>107.5579378834092</v>
+        <v>13.33540149609077</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.7764778809834336</v>
+        <v>0.3882637488404928</v>
       </c>
       <c r="C61" t="n">
-        <v>0.4902207702760648</v>
+        <v>0.7044928928251917</v>
       </c>
       <c r="D61" t="n">
-        <v>50.38558293040208</v>
+        <v>0.8104081229100897</v>
       </c>
       <c r="E61" t="n">
-        <v>63.66944214903458</v>
+        <v>2.215613397653095</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.8502289585388028</v>
+        <v>-0.007079257091528568</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.1712193412313048</v>
+        <v>-0.7945509094096939</v>
       </c>
       <c r="D62" t="n">
-        <v>71.96085284914793</v>
+        <v>3.465349048485524</v>
       </c>
       <c r="E62" t="n">
-        <v>65.43600541793937</v>
+        <v>2.775131704540239</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-0.3042022032960088</v>
+        <v>0.1769636413079536</v>
       </c>
       <c r="C63" t="n">
-        <v>0.07354504957184793</v>
+        <v>-0.2251057327097121</v>
       </c>
       <c r="D63" t="n">
-        <v>9.302915571274884</v>
+        <v>0.1491807483898711</v>
       </c>
       <c r="E63" t="n">
-        <v>6.774823697193709</v>
+        <v>-0.118248165002325</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.009950805174019806</v>
+        <v>-0.0254175353923638</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.6291279088254351</v>
+        <v>0.2169596200201991</v>
       </c>
       <c r="D64" t="n">
-        <v>24.81569611485833</v>
+        <v>-0.07896102132613583</v>
       </c>
       <c r="E64" t="n">
-        <v>9.750890156884221</v>
+        <v>-1.67256002344687</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.9833382283832373</v>
+        <v>0.1423489378910645</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.3783423413227713</v>
+        <v>0.8418371618615739</v>
       </c>
       <c r="D65" t="n">
-        <v>100.114749668311</v>
+        <v>-3.156151344521134</v>
       </c>
       <c r="E65" t="n">
-        <v>83.82617423607451</v>
+        <v>-4.879204241929385</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.6479831944795984</v>
+        <v>-0.8748230754721127</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.695958633561313</v>
+        <v>-0.3063412550757021</v>
       </c>
       <c r="D66" t="n">
-        <v>77.94761436975278</v>
+        <v>9.344244183769776</v>
       </c>
       <c r="E66" t="n">
-        <v>89.01166290641707</v>
+        <v>10.51463142650162</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.4855566405546299</v>
+        <v>0.2270653612477671</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.2454204518165735</v>
+        <v>-0.1642816313342792</v>
       </c>
       <c r="D67" t="n">
-        <v>24.38579654572525</v>
+        <v>0.3290850991904846</v>
       </c>
       <c r="E67" t="n">
-        <v>42.85352408115195</v>
+        <v>2.282655045859172</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.6130735616543666</v>
+        <v>-0.02260512804423387</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.1004527180968482</v>
+        <v>-0.3420060985244866</v>
       </c>
       <c r="D68" t="n">
-        <v>37.30800635585386</v>
+        <v>0.2950621411077129</v>
       </c>
       <c r="E68" t="n">
-        <v>36.3274547741844</v>
+        <v>0.1913365420900075</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.3508849177611184</v>
+        <v>-0.6428520135413482</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7783374612396814</v>
+        <v>-0.9895383810699929</v>
       </c>
       <c r="D69" t="n">
-        <v>-36.09298934142006</v>
+        <v>14.56870486067984</v>
       </c>
       <c r="E69" t="n">
-        <v>-22.42802462965239</v>
+        <v>16.014224583233</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.6050826344410729</v>
+        <v>0.350314859871049</v>
       </c>
       <c r="C70" t="n">
-        <v>0.5954913193746263</v>
+        <v>-0.2240399636297743</v>
       </c>
       <c r="D70" t="n">
-        <v>17.29643519697847</v>
+        <v>0.8476434143319836</v>
       </c>
       <c r="E70" t="n">
-        <v>22.22078150506688</v>
+        <v>1.368555093152036</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.7937274871341833</v>
+        <v>-0.7728239949213842</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.604922686512712</v>
+        <v>-0.4343368549020352</v>
       </c>
       <c r="D71" t="n">
-        <v>82.59577253058087</v>
+        <v>8.439407830286807</v>
       </c>
       <c r="E71" t="n">
-        <v>73.81126860444077</v>
+        <v>7.510157448312082</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.9318892782214903</v>
+        <v>-0.5314496012723968</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.2189184012317049</v>
+        <v>0.7582406655571399</v>
       </c>
       <c r="D72" t="n">
-        <v>88.98227059852407</v>
+        <v>-2.622275642054114</v>
       </c>
       <c r="E72" t="n">
-        <v>93.90334314794809</v>
+        <v>-2.101710270949893</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.391921342757152</v>
+        <v>0.5265769189630509</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3863244750531558</v>
+        <v>0.1426763346521076</v>
       </c>
       <c r="D73" t="n">
-        <v>8.915252996807638</v>
+        <v>3.270207457399977</v>
       </c>
       <c r="E73" t="n">
-        <v>29.85847812705858</v>
+        <v>5.485642741589063</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.9000265212931671</v>
+        <v>-0.2228620205180831</v>
       </c>
       <c r="C74" t="n">
-        <v>0.6292665641489459</v>
+        <v>-0.8187479923669354</v>
       </c>
       <c r="D74" t="n">
-        <v>53.40844880598547</v>
+        <v>5.329244922277868</v>
       </c>
       <c r="E74" t="n">
-        <v>52.92061072790328</v>
+        <v>5.277639991115992</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.6600296796615552</v>
+        <v>-0.03402541977821327</v>
       </c>
       <c r="C75" t="n">
-        <v>0.4780479217095994</v>
+        <v>-0.5548384191565121</v>
       </c>
       <c r="D75" t="n">
-        <v>34.19852837826608</v>
+        <v>1.261594808280535</v>
       </c>
       <c r="E75" t="n">
-        <v>55.50405845914446</v>
+        <v>3.515355764197085</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.7569814979665623</v>
+        <v>0.8443226641224226</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.1348787347145435</v>
+        <v>0.1806096289356347</v>
       </c>
       <c r="D76" t="n">
-        <v>56.94778434729856</v>
+        <v>8.105017461287147</v>
       </c>
       <c r="E76" t="n">
-        <v>21.27508794002613</v>
+        <v>4.331455853114261</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.5423242241084059</v>
+        <v>-0.9036084520916496</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.07977176462247981</v>
+        <v>-0.2722460915797102</v>
       </c>
       <c r="D77" t="n">
-        <v>29.72488549027981</v>
+        <v>9.664768334606826</v>
       </c>
       <c r="E77" t="n">
-        <v>40.9166149715881</v>
+        <v>10.84866203912398</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.1584543565213645</v>
+        <v>-0.1185138497733427</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.4385306621296161</v>
+        <v>0.2015752595497096</v>
       </c>
       <c r="D78" t="n">
-        <v>10.53698985994515</v>
+        <v>-0.0519089607544552</v>
       </c>
       <c r="E78" t="n">
-        <v>11.72229740515472</v>
+        <v>0.0734763197809582</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.791360483413585</v>
+        <v>-0.7571442012099827</v>
       </c>
       <c r="C79" t="n">
-        <v>0.04622812293114253</v>
+        <v>0.07837904097867687</v>
       </c>
       <c r="D79" t="n">
-        <v>62.72366465158368</v>
+        <v>5.305360952487825</v>
       </c>
       <c r="E79" t="n">
-        <v>58.65212409595472</v>
+        <v>4.874661547222006</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.3040918929059917</v>
+        <v>0.5637881824081281</v>
       </c>
       <c r="C80" t="n">
-        <v>0.461986808143529</v>
+        <v>-0.1711069337434368</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1051415322326155</v>
+        <v>2.674098049973682</v>
       </c>
       <c r="E80" t="n">
-        <v>1.354634972772472</v>
+        <v>2.806273101252503</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.8709492337189941</v>
+        <v>0.107169747677079</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.295777627977573</v>
+        <v>-0.2861446214651446</v>
       </c>
       <c r="D81" t="n">
-        <v>79.78840341020046</v>
+        <v>0.07696391574694153</v>
       </c>
       <c r="E81" t="n">
-        <v>52.7239602441829</v>
+        <v>-2.785991620662699</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.04500460018204366</v>
+        <v>-0.954708415140207</v>
       </c>
       <c r="C82" t="n">
-        <v>0.873946197196295</v>
+        <v>0.9507060028930494</v>
       </c>
       <c r="D82" t="n">
-        <v>-66.65265507027559</v>
+        <v>-2.346616255720798</v>
       </c>
       <c r="E82" t="n">
-        <v>-69.64389591725973</v>
+        <v>-2.66303841490125</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.7649911199517176</v>
+        <v>0.1569008628393123</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9901788442878243</v>
+        <v>-0.3730179938528135</v>
       </c>
       <c r="D83" t="n">
-        <v>-42.17322684444788</v>
+        <v>0.236724418293192</v>
       </c>
       <c r="E83" t="n">
-        <v>-37.31047575966812</v>
+        <v>0.7511203751933013</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.4399546182659235</v>
+        <v>-0.3864594987984658</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.4666705362188657</v>
+        <v>-0.347034748942378</v>
       </c>
       <c r="D84" t="n">
-        <v>30.5431200854497</v>
+        <v>2.51741060378579</v>
       </c>
       <c r="E84" t="n">
-        <v>50.66739305302843</v>
+        <v>4.646214745638241</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.3609964991533388</v>
+        <v>0.5594035946020448</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.1779432481848331</v>
+        <v>0.1933058167659285</v>
       </c>
       <c r="D85" t="n">
-        <v>13.93477294802423</v>
+        <v>3.802847573216207</v>
       </c>
       <c r="E85" t="n">
-        <v>6.877561112970335</v>
+        <v>3.056315173829835</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.2891999331675694</v>
+        <v>0.4848911792237589</v>
       </c>
       <c r="C86" t="n">
-        <v>0.2950525656756422</v>
+        <v>-0.7218093469548987</v>
       </c>
       <c r="D86" t="n">
-        <v>6.222281206104896</v>
+        <v>2.859991642646309</v>
       </c>
       <c r="E86" t="n">
-        <v>-4.786861171222569</v>
+        <v>1.695412533187042</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.09355813547180958</v>
+        <v>0.1556265869228493</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.8422753607540172</v>
+        <v>0.04968731595738052</v>
       </c>
       <c r="D87" t="n">
-        <v>60.14107477374224</v>
+        <v>0.3082650537017628</v>
       </c>
       <c r="E87" t="n">
-        <v>53.30872048932764</v>
+        <v>-0.4144812598022071</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.9329830310124321</v>
+        <v>0.6843350602074201</v>
       </c>
       <c r="C88" t="n">
-        <v>0.4637396574672501</v>
+        <v>0.2327929271258942</v>
       </c>
       <c r="D88" t="n">
-        <v>75.04917110725376</v>
+        <v>5.642398224446485</v>
       </c>
       <c r="E88" t="n">
-        <v>87.51407152232929</v>
+        <v>6.960971654360744</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.3941952911831141</v>
+        <v>0.5730998542433208</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.3054126440847185</v>
+        <v>0.1921673804226047</v>
       </c>
       <c r="D89" t="n">
-        <v>17.71586478673328</v>
+        <v>3.972072833522796</v>
       </c>
       <c r="E89" t="n">
-        <v>22.19242188006877</v>
+        <v>4.445616066457691</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.01654486372373842</v>
+        <v>-0.2866426560633117</v>
       </c>
       <c r="C90" t="n">
-        <v>0.8391369335525727</v>
+        <v>-0.3626404712686122</v>
       </c>
       <c r="D90" t="n">
-        <v>-59.0443693405753</v>
+        <v>1.714232321761089</v>
       </c>
       <c r="E90" t="n">
-        <v>-66.25803867357044</v>
+        <v>0.9511493930622901</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-0.3238667439270566</v>
+        <v>0.4230764675883207</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.3786465837140276</v>
+        <v>-0.296899956986485</v>
       </c>
       <c r="D91" t="n">
-        <v>15.23433884503934</v>
+        <v>1.232087569995395</v>
       </c>
       <c r="E91" t="n">
-        <v>22.22342846624301</v>
+        <v>1.971413803413429</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.2431772339480642</v>
+        <v>0.06129620781131528</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8761038239265071</v>
+        <v>-0.1988572702361624</v>
       </c>
       <c r="D92" t="n">
-        <v>-62.28583973568669</v>
+        <v>0.005726546355280165</v>
       </c>
       <c r="E92" t="n">
-        <v>-60.96394855610267</v>
+        <v>0.1455600410961963</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.4548367065342196</v>
+        <v>0.7621092487774721</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.5806123654997133</v>
+        <v>0.2198475235672195</v>
       </c>
       <c r="D93" t="n">
-        <v>41.56854967339385</v>
+        <v>6.837206603804929</v>
       </c>
       <c r="E93" t="n">
-        <v>54.7584507136751</v>
+        <v>8.23247270909037</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.1222383483077731</v>
+        <v>-0.3825593636322742</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4561273334926217</v>
+        <v>-0.2044532983834626</v>
       </c>
       <c r="D94" t="n">
-        <v>-7.683435445852775</v>
+        <v>1.933933225860222</v>
       </c>
       <c r="E94" t="n">
-        <v>-17.2431925537394</v>
+        <v>0.9226743068841807</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.03437538510046245</v>
+        <v>-0.6625741620075234</v>
       </c>
       <c r="C95" t="n">
-        <v>0.0511286610605195</v>
+        <v>0.2597742150488103</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1045635299188433</v>
+        <v>3.194335355873873</v>
       </c>
       <c r="E95" t="n">
-        <v>-4.357165308314329</v>
+        <v>2.722360698903392</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.6001507220594138</v>
+        <v>-0.6010257192536159</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.9336152572300882</v>
+        <v>0.7998164825723955</v>
       </c>
       <c r="D96" t="n">
-        <v>120.1636938914213</v>
+        <v>-2.833597523409672</v>
       </c>
       <c r="E96" t="n">
-        <v>114.8244129500566</v>
+        <v>-3.39840219490278</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>-0.566632787669749</v>
+        <v>0.7271247006657668</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.7461801275835085</v>
+        <v>-0.1784920437626241</v>
       </c>
       <c r="D97" t="n">
-        <v>71.40811371239809</v>
+        <v>4.603057283556583</v>
       </c>
       <c r="E97" t="n">
-        <v>51.47963885783314</v>
+        <v>2.494965235732183</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.2767430925056189</v>
+        <v>-0.9773883453885168</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.5783849106991907</v>
+        <v>0.2196488877269389</v>
       </c>
       <c r="D98" t="n">
-        <v>27.77748853516974</v>
+        <v>8.11483255486023</v>
       </c>
       <c r="E98" t="n">
-        <v>31.80971622299755</v>
+        <v>8.541373330597519</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.5763915516529643</v>
+        <v>0.9425468557563152</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.490263310877219</v>
+        <v>-0.9492662988211975</v>
       </c>
       <c r="D99" t="n">
-        <v>46.42812953435049</v>
+        <v>9.502636282355066</v>
       </c>
       <c r="E99" t="n">
-        <v>49.98288203887967</v>
+        <v>9.878668344089347</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.9863141487899358</v>
+        <v>-0.2291673960669738</v>
       </c>
       <c r="C100" t="n">
-        <v>0.07059867520371355</v>
+        <v>-0.613929522235388</v>
       </c>
       <c r="D100" t="n">
-        <v>97.5029632235005</v>
+        <v>2.904793947748121</v>
       </c>
       <c r="E100" t="n">
-        <v>97.57259243517971</v>
+        <v>2.912159528331103</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.9414831245644188</v>
+        <v>-0.04417557391490567</v>
       </c>
       <c r="C101" t="n">
-        <v>0.2272024584014094</v>
+        <v>0.1380374953700818</v>
       </c>
       <c r="D101" t="n">
-        <v>86.51353870413413</v>
+        <v>-0.02609781139892629</v>
       </c>
       <c r="E101" t="n">
-        <v>83.31919908045093</v>
+        <v>-0.3640043500518034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added expected interval and graphics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6601716109879077</v>
+        <v>-0.9500015408393609</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7420253700032422</v>
+        <v>-0.7809739912525833</v>
       </c>
       <c r="D2" t="n">
-        <v>4.270818430237561</v>
+        <v>16.73785507744002</v>
       </c>
       <c r="E2" t="n">
-        <v>4.986300808699939</v>
+        <v>18.47984701555844</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.6577905566668394</v>
+        <v>0.5886977424584918</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5416984996851222</v>
+        <v>0.1494787886290696</v>
       </c>
       <c r="D3" t="n">
-        <v>1.064648331030498</v>
+        <v>4.038835794358573</v>
       </c>
       <c r="E3" t="n">
-        <v>0.86548816927815</v>
+        <v>3.55393860246331</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.09007713176002641</v>
+        <v>-0.8327916704609981</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2608401713425628</v>
+        <v>0.9708589226610991</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04731675134610744</v>
+        <v>-4.261896595492827</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9802672882570709</v>
+        <v>-1.990432807027762</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8907905122855158</v>
+        <v>0.6302325152994395</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2190924993833352</v>
+        <v>0.8846159827491373</v>
       </c>
       <c r="D5" t="n">
-        <v>9.143441371550756</v>
+        <v>2.65675595787782</v>
       </c>
       <c r="E5" t="n">
-        <v>11.33726052795274</v>
+        <v>7.998068894689659</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.7370357249236463</v>
+        <v>0.3974310597591153</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.6242445150629783</v>
+        <v>-0.2123309065806596</v>
       </c>
       <c r="D6" t="n">
-        <v>9.75942615207256</v>
+        <v>1.173837792633064</v>
       </c>
       <c r="E6" t="n">
-        <v>9.422144412753454</v>
+        <v>0.3526546461926036</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.4362235442361808</v>
+        <v>0.4058245972351495</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4328403625239201</v>
+        <v>0.4883240974364325</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2020296901037268</v>
+        <v>2.10970252545648</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.135228400547366</v>
+        <v>1.288576956659111</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.1375577118130988</v>
+        <v>0.2959819063339824</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.4926364210269423</v>
+        <v>0.1180735661049468</v>
       </c>
       <c r="D8" t="n">
-        <v>1.369705210103058</v>
+        <v>1.11111198107426</v>
       </c>
       <c r="E8" t="n">
-        <v>3.644452032773008</v>
+        <v>6.649460297726623</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3481886954441162</v>
+        <v>-0.2446155472204932</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.9273787197211165</v>
+        <v>-0.515142579919482</v>
       </c>
       <c r="D9" t="n">
-        <v>4.800040969438167</v>
+        <v>2.287687943788707</v>
       </c>
       <c r="E9" t="n">
-        <v>5.905477611418725</v>
+        <v>4.979105337700225</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.6818438902964727</v>
+        <v>0.2107219854290157</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.299516659401097</v>
+        <v>-0.6371758795425684</v>
       </c>
       <c r="D10" t="n">
-        <v>5.964404435176313</v>
+        <v>1.479071548341494</v>
       </c>
       <c r="E10" t="n">
-        <v>5.288159056945047</v>
+        <v>-0.1673896819131784</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.4670435387166465</v>
+        <v>-0.2236221136912659</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1593041632113614</v>
+        <v>-0.4339489445221529</v>
       </c>
       <c r="D11" t="n">
-        <v>2.662043778815145</v>
+        <v>1.629107091655168</v>
       </c>
       <c r="E11" t="n">
-        <v>3.44356399137643</v>
+        <v>3.531881989737355</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.4513216717555475</v>
+        <v>0.5605008666367144</v>
       </c>
       <c r="C12" t="n">
-        <v>0.831354081445655</v>
+        <v>0.7791822247414673</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.198463265009589</v>
+        <v>2.60630105366619</v>
       </c>
       <c r="E12" t="n">
-        <v>-4.865984395754397</v>
+        <v>0.9810808340150476</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.7291312781870849</v>
+        <v>0.3379243143170796</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01938648805631349</v>
+        <v>-0.9630376287753568</v>
       </c>
       <c r="D13" t="n">
-        <v>5.160486957427988</v>
+        <v>5.519837405900468</v>
       </c>
       <c r="E13" t="n">
-        <v>4.489635463092554</v>
+        <v>3.886508717472863</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.6847274588092451</v>
+        <v>0.9344585877533602</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1278197177025777</v>
+        <v>0.7267966922891738</v>
       </c>
       <c r="D14" t="n">
-        <v>4.093078008758599</v>
+        <v>10.30227784525948</v>
       </c>
       <c r="E14" t="n">
-        <v>4.441607923818843</v>
+        <v>11.15084703508749</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.7618079982642816</v>
+        <v>0.5706872590502776</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5964488099618972</v>
+        <v>0.9337122567372458</v>
       </c>
       <c r="D15" t="n">
-        <v>7.180305199118632</v>
+        <v>0.9467279582359585</v>
       </c>
       <c r="E15" t="n">
-        <v>4.424357353030411</v>
+        <v>-5.76320519214832</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2418956531068208</v>
+        <v>-0.4582466843230273</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.8666966550256991</v>
+        <v>0.7685278513095648</v>
       </c>
       <c r="D16" t="n">
-        <v>6.289390533075492</v>
+        <v>-3.138923016660465</v>
       </c>
       <c r="E16" t="n">
-        <v>3.804765712186434</v>
+        <v>-9.188263346382152</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.1308035214710739</v>
+        <v>0.2776637523375207</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6011866037649236</v>
+        <v>-0.7097681420894102</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.774678505797663</v>
+        <v>2.134088659988838</v>
       </c>
       <c r="E17" t="n">
-        <v>-2.584614796845861</v>
+        <v>0.1621288579492364</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.9242029828355653</v>
+        <v>-0.9909812029064653</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3008350840794192</v>
+        <v>0.8280980821773971</v>
       </c>
       <c r="D18" t="n">
-        <v>6.620395946270467</v>
+        <v>0.9324839244412773</v>
       </c>
       <c r="E18" t="n">
-        <v>5.161482777470138</v>
+        <v>-2.619546223284578</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5606838444768714</v>
+        <v>-0.2947657723572066</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4976054088161337</v>
+        <v>-0.7530378434519673</v>
       </c>
       <c r="D19" t="n">
-        <v>4.061000033915709</v>
+        <v>5.1794204955097</v>
       </c>
       <c r="E19" t="n">
-        <v>4.513651579251563</v>
+        <v>6.281495635985524</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.02531840070295654</v>
+        <v>-0.6239097271559741</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08081077221387201</v>
+        <v>0.4168882212978746</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02560505263845424</v>
+        <v>1.800688873643471</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.282340817871755</v>
+        <v>-1.383779717771135</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.1743071937027494</v>
+        <v>-0.3139720675748741</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9578099850724975</v>
+        <v>0.02231134204743235</v>
       </c>
       <c r="D21" t="n">
-        <v>-6.770402710955988</v>
+        <v>0.9134441574824022</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.804728500178554</v>
+        <v>-4.039548719781646</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3768619685565402</v>
+        <v>-0.03240177264604815</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4946252636686568</v>
+        <v>0.3211954874024172</v>
       </c>
       <c r="D22" t="n">
-        <v>1.77874599083716</v>
+        <v>-0.2607652112500316</v>
       </c>
       <c r="E22" t="n">
-        <v>3.889911659907063</v>
+        <v>4.879310472312773</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2514135864542379</v>
+        <v>-0.9810735966778183</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2236662913566698</v>
+        <v>-0.0644172969375989</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9386675050707869</v>
+        <v>9.90520054721414</v>
       </c>
       <c r="E23" t="n">
-        <v>0.613452361726784</v>
+        <v>9.113396059901993</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.8995594822143487</v>
+        <v>-0.3976585483213406</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1885740108469549</v>
+        <v>-0.6726476046290628</v>
       </c>
       <c r="D24" t="n">
-        <v>6.956232785170121</v>
+        <v>5.288473337422495</v>
       </c>
       <c r="E24" t="n">
-        <v>7.053502492929621</v>
+        <v>5.525296845367342</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.9801210197461934</v>
+        <v>-0.1945477105171765</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.5710663792579485</v>
+        <v>-0.6949649440044807</v>
       </c>
       <c r="D25" t="n">
-        <v>7.592633045034922</v>
+        <v>3.533366809805818</v>
       </c>
       <c r="E25" t="n">
-        <v>5.540381836161252</v>
+        <v>-1.463269261839506</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.8182890617882983</v>
+        <v>-0.2427400501527355</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.7034301704556347</v>
+        <v>-0.7083434727907432</v>
       </c>
       <c r="D26" t="n">
-        <v>12.43392294621905</v>
+        <v>4.099252888793832</v>
       </c>
       <c r="E26" t="n">
-        <v>11.64977728784418</v>
+        <v>2.190085792134996</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.4588297104026542</v>
+        <v>0.1293330953001073</v>
       </c>
       <c r="C27" t="n">
-        <v>0.9636195364071038</v>
+        <v>-0.5521224259803543</v>
       </c>
       <c r="D27" t="n">
-        <v>-6.760565131675304</v>
+        <v>0.932795194096656</v>
       </c>
       <c r="E27" t="n">
-        <v>-6.600788813988969</v>
+        <v>1.321804156008466</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.9832528886575727</v>
+        <v>-0.9242903132181204</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.9748654519819226</v>
+        <v>-0.1574212127395409</v>
       </c>
       <c r="D28" t="n">
-        <v>21.70861622349479</v>
+        <v>9.345629163539583</v>
       </c>
       <c r="E28" t="n">
-        <v>20.05068959229931</v>
+        <v>5.309058994276885</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.4306572050387396</v>
+        <v>0.1531075731480609</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7948808672313372</v>
+        <v>-0.3986449466063331</v>
       </c>
       <c r="D29" t="n">
-        <v>-3.678486556270155</v>
+        <v>0.3229386439530511</v>
       </c>
       <c r="E29" t="n">
-        <v>-3.137319548807243</v>
+        <v>1.640523244991037</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.4041124666284004</v>
+        <v>-0.562202911449071</v>
       </c>
       <c r="C30" t="n">
-        <v>0.2497580995677757</v>
+        <v>0.1506632918361275</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9029934372866339</v>
+        <v>2.582144111406183</v>
       </c>
       <c r="E30" t="n">
-        <v>0.03781495212695096</v>
+        <v>0.4756855995688816</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2182710659628795</v>
+        <v>-0.7289913400349486</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.3316322201827497</v>
+        <v>0.9326400710609508</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2860823749864661</v>
+        <v>-4.382907451911507</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.1340822944103889</v>
+        <v>-5.405886478095865</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.1712046574421786</v>
+        <v>0.1315423360431163</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1829034479921863</v>
+        <v>0.5231698495465102</v>
       </c>
       <c r="D32" t="n">
-        <v>0.06356515061768697</v>
+        <v>-0.3497344583042454</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.803151602759568</v>
+        <v>-2.459938206801928</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.02275272003121853</v>
+        <v>0.8074379185633551</v>
       </c>
       <c r="C33" t="n">
-        <v>0.5770044125204641</v>
+        <v>-0.3053627630358655</v>
       </c>
       <c r="D33" t="n">
-        <v>-1.200807986339967</v>
+        <v>5.314309260866783</v>
       </c>
       <c r="E33" t="n">
-        <v>1.467270611767667</v>
+        <v>11.81030629458574</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.119520545724797</v>
+        <v>-0.4733022136158105</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.9286237774343524</v>
+        <v>-0.6493111696374774</v>
       </c>
       <c r="D34" t="n">
-        <v>6.309514678612412</v>
+        <v>5.962706884355584</v>
       </c>
       <c r="E34" t="n">
-        <v>6.29007286001394</v>
+        <v>5.915371698639784</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.2879249668266051</v>
+        <v>-0.8304604385300469</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.2745917802742632</v>
+        <v>0.02588237451346442</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5009009914554854</v>
+        <v>6.685873365975467</v>
       </c>
       <c r="E35" t="n">
-        <v>-1.022658437216371</v>
+        <v>2.976448337654893</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.1848039521941576</v>
+        <v>-0.1604412989019253</v>
       </c>
       <c r="C36" t="n">
-        <v>0.5232229387771894</v>
+        <v>0.4696795644156944</v>
       </c>
       <c r="D36" t="n">
-        <v>-1.207465895251709</v>
+        <v>-0.890497699287356</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.02264684683935458</v>
+        <v>1.994192815242186</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.5381055630462426</v>
+        <v>-0.07373097640829118</v>
       </c>
       <c r="C37" t="n">
-        <v>0.9807847761350361</v>
+        <v>-0.752422360241193</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.3901248881962176</v>
+        <v>3.380674953895479</v>
       </c>
       <c r="E37" t="n">
-        <v>-2.148665717195315</v>
+        <v>-0.9008615859028781</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.8773721693415755</v>
+        <v>-0.1846829579124141</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7930770240696394</v>
+        <v>0.7924610101366609</v>
       </c>
       <c r="D38" t="n">
-        <v>8.548048344577069</v>
+        <v>-3.936719938686909</v>
       </c>
       <c r="E38" t="n">
-        <v>8.848901905568365</v>
+        <v>-3.204228833976055</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.7915404683771203</v>
+        <v>-0.2291665738346753</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.7753419972605025</v>
+        <v>0.6680709614983544</v>
       </c>
       <c r="D39" t="n">
-        <v>5.847401754949177</v>
+        <v>-2.425513696505122</v>
       </c>
       <c r="E39" t="n">
-        <v>3.024632496744735</v>
+        <v>-9.298137591908588</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.8173839988124509</v>
+        <v>0.09983975576003568</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.387482715173709</v>
+        <v>0.2036946580766048</v>
       </c>
       <c r="D40" t="n">
-        <v>8.868256697581579</v>
+        <v>0.1868573797122299</v>
       </c>
       <c r="E40" t="n">
-        <v>6.955096568067598</v>
+        <v>-4.471132281899242</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2029175863657946</v>
+        <v>0.9224463153233646</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.289940625987702</v>
+        <v>0.7389239741660332</v>
       </c>
       <c r="D41" t="n">
-        <v>0.2206670135384639</v>
+        <v>9.958357807076508</v>
       </c>
       <c r="E41" t="n">
-        <v>0.504232006427842</v>
+        <v>10.64875626609583</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.003568278720374574</v>
+        <v>0.4887297383034543</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.5183479187364353</v>
+        <v>-0.5922179701808323</v>
       </c>
       <c r="D42" t="n">
-        <v>0.912456297976264</v>
+        <v>2.160222268712757</v>
       </c>
       <c r="E42" t="n">
-        <v>1.976166324894192</v>
+        <v>4.750047465203171</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.5782020891481092</v>
+        <v>-0.5333445231465146</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2707970143937481</v>
+        <v>-0.4487056200098953</v>
       </c>
       <c r="D43" t="n">
-        <v>4.228524111407247</v>
+        <v>4.857202319982068</v>
       </c>
       <c r="E43" t="n">
-        <v>4.475368266492228</v>
+        <v>5.458196196384434</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.6310925033788195</v>
+        <v>0.8735797033932173</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.7930132509468328</v>
+        <v>-0.8932554644629931</v>
       </c>
       <c r="D44" t="n">
-        <v>4.454712888599015</v>
+        <v>8.061054689669826</v>
       </c>
       <c r="E44" t="n">
-        <v>4.288129537497368</v>
+        <v>7.655472576987401</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.9470700010447128</v>
+        <v>0.2201586352005902</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.7042774474384761</v>
+        <v>-0.787804338661146</v>
       </c>
       <c r="D45" t="n">
-        <v>7.436979308222686</v>
+        <v>2.911312240732089</v>
       </c>
       <c r="E45" t="n">
-        <v>7.003260262815972</v>
+        <v>1.855332242831079</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.05258332140162891</v>
+        <v>0.2142758418819022</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1475369495572014</v>
+        <v>-0.02289733694218121</v>
       </c>
       <c r="D46" t="n">
-        <v>0.07172976710108911</v>
+        <v>0.4501224669853214</v>
       </c>
       <c r="E46" t="n">
-        <v>-2.05797888698893</v>
+        <v>-4.73510000339718</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.8208058171760202</v>
+        <v>-0.7162182654315072</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9100892663500566</v>
+        <v>-0.7273667203878345</v>
       </c>
       <c r="D47" t="n">
-        <v>6.115801284233272</v>
+        <v>10.89407849832723</v>
       </c>
       <c r="E47" t="n">
-        <v>5.078915495450509</v>
+        <v>8.369562536535296</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.6143533084408594</v>
+        <v>0.7899638676267338</v>
       </c>
       <c r="C48" t="n">
-        <v>0.744224731851771</v>
+        <v>0.7840057246544316</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.841443156893109</v>
+        <v>6.762803438022819</v>
       </c>
       <c r="E48" t="n">
-        <v>-2.504961442934059</v>
+        <v>5.147328983485623</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.579526041185098</v>
+        <v>0.8133754035333005</v>
       </c>
       <c r="C49" t="n">
-        <v>0.09893055218341895</v>
+        <v>0.3715206653148468</v>
       </c>
       <c r="D49" t="n">
-        <v>3.763569161802632</v>
+        <v>8.183665678397498</v>
       </c>
       <c r="E49" t="n">
-        <v>5.286280604903891</v>
+        <v>11.89102610796332</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.2882188581859915</v>
+        <v>-0.2453592819881485</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.4044455032943419</v>
+        <v>0.6173373014164267</v>
       </c>
       <c r="D50" t="n">
-        <v>1.923951103984979</v>
+        <v>-1.909257189431692</v>
       </c>
       <c r="E50" t="n">
-        <v>2.418909481178747</v>
+        <v>-0.7041771920337443</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.3475433568596666</v>
+        <v>0.7012865141166289</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8375466603904462</v>
+        <v>-0.6730569183518755</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.039805946626231</v>
+        <v>4.302059619612407</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.579343336564632</v>
+        <v>-1.880976878547278</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.02171678191628401</v>
+        <v>0.9178848709480312</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9390481360720671</v>
+        <v>0.3719650736818469</v>
       </c>
       <c r="D52" t="n">
-        <v>-5.822352772885137</v>
+        <v>10.23762514004416</v>
       </c>
       <c r="E52" t="n">
-        <v>-5.355532232664144</v>
+        <v>11.37419767081797</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3214996916734061</v>
+        <v>0.6242100604466096</v>
       </c>
       <c r="C53" t="n">
-        <v>0.4140725541779864</v>
+        <v>-0.4369900940233808</v>
       </c>
       <c r="D53" t="n">
-        <v>1.408956133855417</v>
+        <v>2.903542298646212</v>
       </c>
       <c r="E53" t="n">
-        <v>0.8542717460124317</v>
+        <v>1.553046799512912</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.1396449706657175</v>
+        <v>0.1158408561705357</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2675229462784174</v>
+        <v>0.3166985393699402</v>
       </c>
       <c r="D54" t="n">
-        <v>0.3258498119042283</v>
+        <v>0.1694100955799742</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.6492095051623128</v>
+        <v>-2.204576351392289</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.3634220280899987</v>
+        <v>-0.6523656644728719</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1865768499600544</v>
+        <v>0.8564204433955587</v>
       </c>
       <c r="D55" t="n">
-        <v>0.8507699801410415</v>
+        <v>-3.442482939038026</v>
       </c>
       <c r="E55" t="n">
-        <v>1.731847363049855</v>
+        <v>-1.297315225496172</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.8366308697459344</v>
+        <v>-0.4916982412589268</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9072398542264835</v>
+        <v>0.3175064958195442</v>
       </c>
       <c r="D56" t="n">
-        <v>6.500905174871431</v>
+        <v>1.233698187118806</v>
       </c>
       <c r="E56" t="n">
-        <v>7.985988670231985</v>
+        <v>4.849445484641997</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.014873089059388</v>
+        <v>-0.8520082559366475</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.8711755234133918</v>
+        <v>-0.6713753143632599</v>
       </c>
       <c r="D57" t="n">
-        <v>4.619580738381517</v>
+        <v>12.73592201826065</v>
       </c>
       <c r="E57" t="n">
-        <v>5.961025331012072</v>
+        <v>16.00195027575162</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.9687245970242016</v>
+        <v>0.9349203932330696</v>
       </c>
       <c r="C58" t="n">
-        <v>0.7015387762096723</v>
+        <v>0.02828647538644846</v>
       </c>
       <c r="D58" t="n">
-        <v>2.863098817196008</v>
+        <v>8.994262979589832</v>
       </c>
       <c r="E58" t="n">
-        <v>1.654264025751962</v>
+        <v>6.051101100833213</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.8481490587914116</v>
+        <v>0.0632052145628339</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.06535188174948203</v>
+        <v>-0.204943322596109</v>
       </c>
       <c r="D59" t="n">
-        <v>6.941232920043901</v>
+        <v>0.02275747288797615</v>
       </c>
       <c r="E59" t="n">
-        <v>6.495833881617414</v>
+        <v>-1.061659918148347</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.9488575920651898</v>
+        <v>0.6980158272434187</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.5250434561016888</v>
+        <v>0.297014340531804</v>
       </c>
       <c r="D60" t="n">
-        <v>12.85823943746735</v>
+        <v>6.026246189552989</v>
       </c>
       <c r="E60" t="n">
-        <v>13.33540149609077</v>
+        <v>7.187997316232487</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.3882637488404928</v>
+        <v>-0.8148474128801571</v>
       </c>
       <c r="C61" t="n">
-        <v>0.7044928928251917</v>
+        <v>-0.9023543851846412</v>
       </c>
       <c r="D61" t="n">
-        <v>0.8104081229100897</v>
+        <v>16.14942471198119</v>
       </c>
       <c r="E61" t="n">
-        <v>2.215613397653095</v>
+        <v>19.5706917252435</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.007079257091528568</v>
+        <v>-0.3534701079038041</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.7945509094096939</v>
+        <v>0.07427862891395276</v>
       </c>
       <c r="D62" t="n">
-        <v>3.465349048485524</v>
+        <v>1.057929444073597</v>
       </c>
       <c r="E62" t="n">
-        <v>2.775131704540239</v>
+        <v>-0.6225494676308909</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.1769636413079536</v>
+        <v>-0.0468452175873435</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.2251057327097121</v>
+        <v>-0.1880717868650645</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1491807483898711</v>
+        <v>0.1108213216561033</v>
       </c>
       <c r="E63" t="n">
-        <v>-0.118248165002325</v>
+        <v>-0.5402904669390795</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.0254175353923638</v>
+        <v>0.5899325039189485</v>
       </c>
       <c r="C64" t="n">
-        <v>0.2169596200201991</v>
+        <v>-0.5822832412077825</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.07896102132613583</v>
+        <v>2.864918503745249</v>
       </c>
       <c r="E64" t="n">
-        <v>-1.67256002344687</v>
+        <v>-1.015032558437126</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.1423489378910645</v>
+        <v>-0.07544379184167416</v>
       </c>
       <c r="C65" t="n">
-        <v>0.8418371618615739</v>
+        <v>0.6766367999504472</v>
       </c>
       <c r="D65" t="n">
-        <v>-3.156151344521134</v>
+        <v>-2.345826659998838</v>
       </c>
       <c r="E65" t="n">
-        <v>-4.879204241929385</v>
+        <v>-6.540960385985614</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.8748230754721127</v>
+        <v>-0.08389443755851578</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.3063412550757021</v>
+        <v>-0.8956979593408458</v>
       </c>
       <c r="D66" t="n">
-        <v>9.344244183769776</v>
+        <v>5.57847189118719</v>
       </c>
       <c r="E66" t="n">
-        <v>10.51463142650162</v>
+        <v>8.428025147407217</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.2270653612477671</v>
+        <v>0.001636286842523926</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.1642816313342792</v>
+        <v>-0.0182034893296581</v>
       </c>
       <c r="D67" t="n">
-        <v>0.3290850991904846</v>
+        <v>-0.0008231272614412924</v>
       </c>
       <c r="E67" t="n">
-        <v>2.282655045859172</v>
+        <v>4.755552711037734</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.02260512804423387</v>
+        <v>-0.9111679078929076</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.3420060985244866</v>
+        <v>0.5453917175382152</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2950621411077129</v>
+        <v>4.150911510365241</v>
       </c>
       <c r="E68" t="n">
-        <v>0.1913365420900075</v>
+        <v>3.89836978089084</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.6428520135413482</v>
+        <v>-0.7600597095964494</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.9895383810699929</v>
+        <v>0.5487656138990866</v>
       </c>
       <c r="D69" t="n">
-        <v>14.56870486067984</v>
+        <v>2.099085354366048</v>
       </c>
       <c r="E69" t="n">
-        <v>16.014224583233</v>
+        <v>5.618506347641002</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.350314859871049</v>
+        <v>0.2424885704097766</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.2240399636297743</v>
+        <v>-0.4877024087308801</v>
       </c>
       <c r="D70" t="n">
-        <v>0.8476434143319836</v>
+        <v>0.7140951593801728</v>
       </c>
       <c r="E70" t="n">
-        <v>1.368555093152036</v>
+        <v>1.982363913848143</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.7728239949213842</v>
+        <v>-0.4196417329932465</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.4343368549020352</v>
+        <v>0.7694732782785458</v>
       </c>
       <c r="D71" t="n">
-        <v>8.439407830286807</v>
+        <v>-3.309885681655851</v>
       </c>
       <c r="E71" t="n">
-        <v>7.510157448312082</v>
+        <v>-5.572340666741902</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.5314496012723968</v>
+        <v>0.3232178325095465</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7582406655571399</v>
+        <v>0.1940766609461633</v>
       </c>
       <c r="D72" t="n">
-        <v>-2.622275642054114</v>
+        <v>1.415693788618198</v>
       </c>
       <c r="E72" t="n">
-        <v>-2.101710270949893</v>
+        <v>2.683119384306519</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.5265769189630509</v>
+        <v>0.9473741778635432</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1426763346521076</v>
+        <v>-0.4481375245890176</v>
       </c>
       <c r="D73" t="n">
-        <v>3.270207457399977</v>
+        <v>7.15025563930291</v>
       </c>
       <c r="E73" t="n">
-        <v>5.485642741589063</v>
+        <v>12.54419757365819</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.2228620205180831</v>
+        <v>0.6123772671915659</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.8187479923669354</v>
+        <v>0.8035015327638362</v>
       </c>
       <c r="D74" t="n">
-        <v>5.329244922277868</v>
+        <v>3.237043004153821</v>
       </c>
       <c r="E74" t="n">
-        <v>5.277639991115992</v>
+        <v>3.111399974000744</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.03402541977821327</v>
+        <v>-0.7674533247388757</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.5548384191565121</v>
+        <v>0.1884938425944132</v>
       </c>
       <c r="D75" t="n">
-        <v>1.261594808280535</v>
+        <v>4.911236842392533</v>
       </c>
       <c r="E75" t="n">
-        <v>3.515355764197085</v>
+        <v>10.39849066419876</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.8443226641224226</v>
+        <v>0.6658713463743373</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1806096289356347</v>
+        <v>0.7011277510178788</v>
       </c>
       <c r="D76" t="n">
-        <v>8.105017461287147</v>
+        <v>4.973190047238177</v>
       </c>
       <c r="E76" t="n">
-        <v>4.331455853114261</v>
+        <v>-4.214337273221183</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.9036084520916496</v>
+        <v>-0.1608952273584701</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.2722460915797102</v>
+        <v>0.2164526834376199</v>
       </c>
       <c r="D77" t="n">
-        <v>9.664768334606826</v>
+        <v>-0.02165452310883521</v>
       </c>
       <c r="E77" t="n">
-        <v>10.84866203912398</v>
+        <v>2.860783047597149</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.1185138497733427</v>
+        <v>-0.5389561860740291</v>
       </c>
       <c r="C78" t="n">
-        <v>0.2015752595497096</v>
+        <v>0.1939523271833545</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.0519089607544552</v>
+        <v>2.186038595353307</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0734763197809582</v>
+        <v>2.491315363064633</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.7571442012099827</v>
+        <v>0.8474286898932315</v>
       </c>
       <c r="C79" t="n">
-        <v>0.07837904097867687</v>
+        <v>-0.5658306806068001</v>
       </c>
       <c r="D79" t="n">
-        <v>5.305360952487825</v>
+        <v>5.660926421776411</v>
       </c>
       <c r="E79" t="n">
-        <v>4.874661547222006</v>
+        <v>4.612298371232599</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.5637881824081281</v>
+        <v>-0.2636027265603627</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.1711069337434368</v>
+        <v>-0.09262916008048472</v>
       </c>
       <c r="D80" t="n">
-        <v>2.674098049973682</v>
+        <v>0.8167974668477203</v>
       </c>
       <c r="E80" t="n">
-        <v>2.806273101252503</v>
+        <v>1.138605355733697</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.107169747677079</v>
+        <v>-0.06024439160063655</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.2861446214651446</v>
+        <v>-0.2435609393679155</v>
       </c>
       <c r="D81" t="n">
-        <v>0.07696391574694153</v>
+        <v>0.213202194835919</v>
       </c>
       <c r="E81" t="n">
-        <v>-2.785991620662699</v>
+        <v>-6.757263624790593</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.954708415140207</v>
+        <v>0.05612212829982499</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9507060028930494</v>
+        <v>0.4778171991243123</v>
       </c>
       <c r="D82" t="n">
-        <v>-2.346616255720798</v>
+        <v>-0.5189030486759382</v>
       </c>
       <c r="E82" t="n">
-        <v>-2.66303841490125</v>
+        <v>-1.289299171525181</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.1569008628393123</v>
+        <v>0.8108416400785676</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.3730179938528135</v>
+        <v>-0.8869769931459679</v>
       </c>
       <c r="D83" t="n">
-        <v>0.236724418293192</v>
+        <v>7.259531115023133</v>
       </c>
       <c r="E83" t="n">
-        <v>0.7511203751933013</v>
+        <v>8.511935977664789</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-0.3864594987984658</v>
+        <v>-0.2556362406834507</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.347034748942378</v>
+        <v>0.8127133919933154</v>
       </c>
       <c r="D84" t="n">
-        <v>2.51741060378579</v>
+        <v>-4.269530513025366</v>
       </c>
       <c r="E84" t="n">
-        <v>4.646214745638241</v>
+        <v>0.9134897325739635</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.5594035946020448</v>
+        <v>0.5206123817010497</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1933058167659285</v>
+        <v>-0.3050008883360609</v>
       </c>
       <c r="D85" t="n">
-        <v>3.802847573216207</v>
+        <v>2.002372944752598</v>
       </c>
       <c r="E85" t="n">
-        <v>3.056315173829835</v>
+        <v>0.1847832172878554</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.4848911792237589</v>
+        <v>-0.06108915088516498</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.7218093469548987</v>
+        <v>0.9975662935676457</v>
       </c>
       <c r="D86" t="n">
-        <v>2.859991642646309</v>
+        <v>-7.13405721828433</v>
       </c>
       <c r="E86" t="n">
-        <v>1.695412533187042</v>
+        <v>-9.969469355671922</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.1556265869228493</v>
+        <v>0.5910410700261139</v>
       </c>
       <c r="C87" t="n">
-        <v>0.04968731595738052</v>
+        <v>0.1927056478240021</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3082650537017628</v>
+        <v>4.199036615202018</v>
       </c>
       <c r="E87" t="n">
-        <v>-0.4144812598022071</v>
+        <v>2.439359103458903</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.6843350602074201</v>
+        <v>-0.9624215880365719</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2327929271258942</v>
+        <v>0.1118075462146098</v>
       </c>
       <c r="D88" t="n">
-        <v>5.642398224446485</v>
+        <v>8.517731579221875</v>
       </c>
       <c r="E88" t="n">
-        <v>6.960971654360744</v>
+        <v>11.72807519336383</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5730998542433208</v>
+        <v>-0.2385001518372951</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1921673804226047</v>
+        <v>-0.8118905315607421</v>
       </c>
       <c r="D89" t="n">
-        <v>3.972072833522796</v>
+        <v>5.478307172140977</v>
       </c>
       <c r="E89" t="n">
-        <v>4.445616066457691</v>
+        <v>6.631247508555559</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-0.2866426560633117</v>
+        <v>0.3273627686782998</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.3626404712686122</v>
+        <v>0.3697307081202754</v>
       </c>
       <c r="D90" t="n">
-        <v>1.714232321761089</v>
+        <v>1.508975748643582</v>
       </c>
       <c r="E90" t="n">
-        <v>0.9511493930622901</v>
+        <v>-0.3489097142602369</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.4230764675883207</v>
+        <v>-0.5067524010892728</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.296899956986485</v>
+        <v>-0.4006067858621802</v>
       </c>
       <c r="D91" t="n">
-        <v>1.232087569995395</v>
+        <v>4.181415559002277</v>
       </c>
       <c r="E91" t="n">
-        <v>1.971413803413429</v>
+        <v>5.981460363769459</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.06129620781131528</v>
+        <v>-0.3087748489220747</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.1988572702361624</v>
+        <v>0.8114461266907913</v>
       </c>
       <c r="D92" t="n">
-        <v>0.005726546355280165</v>
+        <v>-4.214414026743059</v>
       </c>
       <c r="E92" t="n">
-        <v>0.1455600410961963</v>
+        <v>-3.873960050726082</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.7621092487774721</v>
+        <v>0.08520766465288943</v>
       </c>
       <c r="C93" t="n">
-        <v>0.2198475235672195</v>
+        <v>-0.8522363668452089</v>
       </c>
       <c r="D93" t="n">
-        <v>6.837206603804929</v>
+        <v>4.008336296581703</v>
       </c>
       <c r="E93" t="n">
-        <v>8.23247270909037</v>
+        <v>7.405404316845918</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.3825593636322742</v>
+        <v>0.8735825906540495</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.2044532983834626</v>
+        <v>-0.2819348971342956</v>
       </c>
       <c r="D94" t="n">
-        <v>1.933933225860222</v>
+        <v>6.391786841814779</v>
       </c>
       <c r="E94" t="n">
-        <v>0.9226743068841807</v>
+        <v>3.92966487035208</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.6625741620075234</v>
+        <v>0.8036314689319155</v>
       </c>
       <c r="C95" t="n">
-        <v>0.2597742150488103</v>
+        <v>-0.1698072039250533</v>
       </c>
       <c r="D95" t="n">
-        <v>3.194335355873873</v>
+        <v>5.748491262281052</v>
       </c>
       <c r="E95" t="n">
-        <v>2.722360698903392</v>
+        <v>4.599369953094237</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.6010257192536159</v>
+        <v>-0.7577902070698057</v>
       </c>
       <c r="C96" t="n">
-        <v>0.7998164825723955</v>
+        <v>0.8231234913476653</v>
       </c>
       <c r="D96" t="n">
-        <v>-2.833597523409672</v>
+        <v>-1.870788326616345</v>
       </c>
       <c r="E96" t="n">
-        <v>-3.39840219490278</v>
+        <v>-3.245923779242101</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.7271247006657668</v>
+        <v>-0.5926137079605509</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.1784920437626241</v>
+        <v>-0.7093485566815232</v>
       </c>
       <c r="D97" t="n">
-        <v>4.603057283556583</v>
+        <v>8.488203959385997</v>
       </c>
       <c r="E97" t="n">
-        <v>2.494965235732183</v>
+        <v>3.355611651503252</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.9773883453885168</v>
+        <v>0.3560747762835001</v>
       </c>
       <c r="C98" t="n">
-        <v>0.2196488877269389</v>
+        <v>0.377103244443177</v>
       </c>
       <c r="D98" t="n">
-        <v>8.11483255486023</v>
+        <v>1.766850838989188</v>
       </c>
       <c r="E98" t="n">
-        <v>8.541373330597519</v>
+        <v>2.805353833584187</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.9425468557563152</v>
+        <v>0.08563252738979732</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.9492662988211975</v>
+        <v>0.1778981903406467</v>
       </c>
       <c r="D99" t="n">
-        <v>9.502636282355066</v>
+        <v>0.1459449040263786</v>
       </c>
       <c r="E99" t="n">
-        <v>9.878668344089347</v>
+        <v>1.061473839096591</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.2291673960669738</v>
+        <v>-0.8777626389173576</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.613929522235388</v>
+        <v>0.0103432200561846</v>
       </c>
       <c r="D100" t="n">
-        <v>2.904793947748121</v>
+        <v>7.562942999551167</v>
       </c>
       <c r="E100" t="n">
-        <v>2.912159528331103</v>
+        <v>7.580876050568707</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,356 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-0.04417557391490567</v>
+        <v>0.2396460651098011</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1380374953700818</v>
+        <v>-0.1585097153828838</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.02609781139892629</v>
+        <v>0.3928149037229367</v>
       </c>
       <c r="E101" t="n">
-        <v>-0.3640043500518034</v>
+        <v>-0.4298894477606315</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.2569140295572936</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-0.5522380718853928</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1.016258407740441</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-3.947490676422959</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.5110713096728339</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-0.5156171394893854</v>
+      </c>
+      <c r="D103" t="n">
+        <v>2.042325995442948</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.5671098039528204</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.1348822000823553</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-0.1576985184576765</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.08985035212774523</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-1.112060085186255</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.1233522060269385</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-0.1309104877596889</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.07847693489558892</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-2.735134327532272</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.6437527207506866</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-0.8805165212951429</v>
+      </c>
+      <c r="D106" t="n">
+        <v>12.2930237357572</v>
+      </c>
+      <c r="E106" t="n">
+        <v>11.72738974334401</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-0.01553137907953261</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.3657315263414935</v>
+      </c>
+      <c r="D107" t="n">
+        <v>-0.3440008482069073</v>
+      </c>
+      <c r="E107" t="n">
+        <v>1.073018036585869</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.3556437166039661</v>
+      </c>
+      <c r="C108" t="n">
+        <v>-0.5672255257758296</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1.371333973713971</v>
+      </c>
+      <c r="E108" t="n">
+        <v>7.986246421411155</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.8985914391221863</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.7355907932421841</v>
+      </c>
+      <c r="D109" t="n">
+        <v>9.435221946059896</v>
+      </c>
+      <c r="E109" t="n">
+        <v>10.04747174946047</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.955383002168303</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-0.2657645786235827</v>
+      </c>
+      <c r="D110" t="n">
+        <v>7.824836369289282</v>
+      </c>
+      <c r="E110" t="n">
+        <v>8.728073576400146</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-0.4494435471441012</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-0.8997601917345204</v>
+      </c>
+      <c r="D111" t="n">
+        <v>9.536289917778847</v>
+      </c>
+      <c r="E111" t="n">
+        <v>9.275205782558778</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.5080278033687873</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.5001167197137582</v>
+      </c>
+      <c r="D112" t="n">
+        <v>3.330569049323524</v>
+      </c>
+      <c r="E112" t="n">
+        <v>-3.39862110537904</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-0.08809168402310874</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.7576455846705414</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-3.28073867378473</v>
+      </c>
+      <c r="E113" t="n">
+        <v>-3.373723657201877</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>-0.6762615228396922</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-0.25182823629073</v>
+      </c>
+      <c r="D114" t="n">
+        <v>5.63302328486217</v>
+      </c>
+      <c r="E114" t="n">
+        <v>5.844252498912923</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-0.6427670815072206</v>
+      </c>
+      <c r="C115" t="n">
+        <v>-0.2314892998838534</v>
+      </c>
+      <c r="D115" t="n">
+        <v>5.040599176635528</v>
+      </c>
+      <c r="E115" t="n">
+        <v>13.67926565225358</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.1705263900264247</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-0.3134046715439769</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.1968182541080766</v>
+      </c>
+      <c r="E116" t="n">
+        <v>-0.4777976146485736</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.1509461650735722</v>
+      </c>
+      <c r="C117" t="n">
+        <v>-0.4648973256172411</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1.335513989580544</v>
+      </c>
+      <c r="E117" t="n">
+        <v>2.393049870371741</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-0.9765363498987523</v>
+      </c>
+      <c r="C118" t="n">
+        <v>-0.8707918067892928</v>
+      </c>
+      <c r="D118" t="n">
+        <v>19.19514430135876</v>
+      </c>
+      <c r="E118" t="n">
+        <v>19.07340904856239</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-0.07818722260458677</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-0.06478115879848834</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.08278767435358945</v>
+      </c>
+      <c r="E119" t="n">
+        <v>-4.015802445230219</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.1009793474979794</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-0.960306916634506</v>
+      </c>
+      <c r="D120" t="n">
+        <v>5.773536658513576</v>
+      </c>
+      <c r="E120" t="n">
+        <v>9.781451708878462</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.1373826693855262</v>
+      </c>
+      <c r="C121" t="n">
+        <v>-0.7534370809704694</v>
+      </c>
+      <c r="D121" t="n">
+        <v>2.594429816696655</v>
+      </c>
+      <c r="E121" t="n">
+        <v>5.231482280381281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>